<commit_message>
Transferring data from pdfs to xlsx
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009831A2-2377-445F-986B-32708D552EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B0C386-B7F2-4D1C-903F-99522A760CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="195" windowWidth="9900" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="59">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t>21/6/2020</t>
+  </si>
+  <si>
+    <t>22/6/2020</t>
+  </si>
+  <si>
+    <t>23/6/2020</t>
+  </si>
+  <si>
+    <t>24/6/2020</t>
   </si>
 </sst>
 </file>
@@ -560,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D193"/>
+  <dimension ref="A1:D289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="D193" sqref="D193"/>
+    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
+      <selection activeCell="D290" sqref="D290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3276,6 +3285,1350 @@
         <v>139</v>
       </c>
     </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>56</v>
+      </c>
+      <c r="B194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194">
+        <v>672.94</v>
+      </c>
+      <c r="D194">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>56</v>
+      </c>
+      <c r="B195" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195">
+        <v>252.86</v>
+      </c>
+      <c r="D195">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>56</v>
+      </c>
+      <c r="B196" t="s">
+        <v>7</v>
+      </c>
+      <c r="C196">
+        <v>19.8</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>56</v>
+      </c>
+      <c r="B197" t="s">
+        <v>8</v>
+      </c>
+      <c r="C197">
+        <v>234.7</v>
+      </c>
+      <c r="D197">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>56</v>
+      </c>
+      <c r="B198" t="s">
+        <v>9</v>
+      </c>
+      <c r="C198">
+        <v>31.59</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>56</v>
+      </c>
+      <c r="B199" t="s">
+        <v>10</v>
+      </c>
+      <c r="C199">
+        <v>284.02999999999997</v>
+      </c>
+      <c r="D199">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>56</v>
+      </c>
+      <c r="B200" t="s">
+        <v>11</v>
+      </c>
+      <c r="C200">
+        <v>63.09</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>56</v>
+      </c>
+      <c r="B201" t="s">
+        <v>12</v>
+      </c>
+      <c r="C201">
+        <v>37.43</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>56</v>
+      </c>
+      <c r="B202" t="s">
+        <v>13</v>
+      </c>
+      <c r="C202">
+        <v>290.60000000000002</v>
+      </c>
+      <c r="D202">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>56</v>
+      </c>
+      <c r="B203" t="s">
+        <v>14</v>
+      </c>
+      <c r="C203">
+        <v>118.1</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>56</v>
+      </c>
+      <c r="B204" t="s">
+        <v>15</v>
+      </c>
+      <c r="C204">
+        <v>188.73</v>
+      </c>
+      <c r="D204">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>56</v>
+      </c>
+      <c r="B205" t="s">
+        <v>16</v>
+      </c>
+      <c r="C205">
+        <v>267.79000000000002</v>
+      </c>
+      <c r="D205">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>56</v>
+      </c>
+      <c r="B206" t="s">
+        <v>17</v>
+      </c>
+      <c r="C206">
+        <v>284.23</v>
+      </c>
+      <c r="D206">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>56</v>
+      </c>
+      <c r="B207" t="s">
+        <v>18</v>
+      </c>
+      <c r="C207">
+        <v>136.08000000000001</v>
+      </c>
+      <c r="D207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>56</v>
+      </c>
+      <c r="B208" t="s">
+        <v>19</v>
+      </c>
+      <c r="C208">
+        <v>39.24</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>56</v>
+      </c>
+      <c r="B209" t="s">
+        <v>20</v>
+      </c>
+      <c r="C209">
+        <v>128.58000000000001</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>56</v>
+      </c>
+      <c r="B210" t="s">
+        <v>21</v>
+      </c>
+      <c r="C210">
+        <v>82.56</v>
+      </c>
+      <c r="D210">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>56</v>
+      </c>
+      <c r="B211" t="s">
+        <v>22</v>
+      </c>
+      <c r="C211">
+        <v>130.24</v>
+      </c>
+      <c r="D211">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>56</v>
+      </c>
+      <c r="B212" t="s">
+        <v>23</v>
+      </c>
+      <c r="C212">
+        <v>281.07</v>
+      </c>
+      <c r="D212">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>56</v>
+      </c>
+      <c r="B213" t="s">
+        <v>24</v>
+      </c>
+      <c r="C213">
+        <v>57.95</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>56</v>
+      </c>
+      <c r="B214" t="s">
+        <v>25</v>
+      </c>
+      <c r="C214">
+        <v>270.3</v>
+      </c>
+      <c r="D214">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>56</v>
+      </c>
+      <c r="B215" t="s">
+        <v>26</v>
+      </c>
+      <c r="C215">
+        <v>113.65</v>
+      </c>
+      <c r="D215">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>56</v>
+      </c>
+      <c r="B216" t="s">
+        <v>27</v>
+      </c>
+      <c r="C216">
+        <v>77.06</v>
+      </c>
+      <c r="D216">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>56</v>
+      </c>
+      <c r="B217" t="s">
+        <v>28</v>
+      </c>
+      <c r="C217">
+        <v>192.79</v>
+      </c>
+      <c r="D217">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>56</v>
+      </c>
+      <c r="B218" t="s">
+        <v>29</v>
+      </c>
+      <c r="C218">
+        <v>185.23</v>
+      </c>
+      <c r="D218">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>56</v>
+      </c>
+      <c r="B219" t="s">
+        <v>30</v>
+      </c>
+      <c r="C219">
+        <v>123.98</v>
+      </c>
+      <c r="D219">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>56</v>
+      </c>
+      <c r="B220" t="s">
+        <v>31</v>
+      </c>
+      <c r="C220">
+        <v>99.59</v>
+      </c>
+      <c r="D220">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>56</v>
+      </c>
+      <c r="B221" t="s">
+        <v>32</v>
+      </c>
+      <c r="C221">
+        <v>226.08</v>
+      </c>
+      <c r="D221">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>56</v>
+      </c>
+      <c r="B222" t="s">
+        <v>33</v>
+      </c>
+      <c r="C222">
+        <v>28.27</v>
+      </c>
+      <c r="D222">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>56</v>
+      </c>
+      <c r="B223" t="s">
+        <v>34</v>
+      </c>
+      <c r="C223">
+        <v>20.99</v>
+      </c>
+      <c r="D223">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>56</v>
+      </c>
+      <c r="B224" t="s">
+        <v>35</v>
+      </c>
+      <c r="C224">
+        <v>95.58</v>
+      </c>
+      <c r="D224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>56</v>
+      </c>
+      <c r="B225" t="s">
+        <v>36</v>
+      </c>
+      <c r="C225">
+        <v>285.10000000000002</v>
+      </c>
+      <c r="D225">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>57</v>
+      </c>
+      <c r="B226" t="s">
+        <v>5</v>
+      </c>
+      <c r="C226">
+        <v>687.32</v>
+      </c>
+      <c r="D226">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>57</v>
+      </c>
+      <c r="B227" t="s">
+        <v>6</v>
+      </c>
+      <c r="C227">
+        <v>259.16000000000003</v>
+      </c>
+      <c r="D227">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>57</v>
+      </c>
+      <c r="B228" t="s">
+        <v>7</v>
+      </c>
+      <c r="C228">
+        <v>19.8</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>57</v>
+      </c>
+      <c r="B229" t="s">
+        <v>8</v>
+      </c>
+      <c r="C229">
+        <v>236.82</v>
+      </c>
+      <c r="D229">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>57</v>
+      </c>
+      <c r="B230" t="s">
+        <v>9</v>
+      </c>
+      <c r="C230">
+        <v>31.59</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>57</v>
+      </c>
+      <c r="B231" t="s">
+        <v>10</v>
+      </c>
+      <c r="C231">
+        <v>284.7</v>
+      </c>
+      <c r="D231">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>57</v>
+      </c>
+      <c r="B232" t="s">
+        <v>11</v>
+      </c>
+      <c r="C232">
+        <v>72.55</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>57</v>
+      </c>
+      <c r="B233" t="s">
+        <v>12</v>
+      </c>
+      <c r="C233">
+        <v>38.5</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>57</v>
+      </c>
+      <c r="B234" t="s">
+        <v>13</v>
+      </c>
+      <c r="C234">
+        <v>301.44</v>
+      </c>
+      <c r="D234">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>57</v>
+      </c>
+      <c r="B235" t="s">
+        <v>14</v>
+      </c>
+      <c r="C235">
+        <v>118.1</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>57</v>
+      </c>
+      <c r="B236" t="s">
+        <v>15</v>
+      </c>
+      <c r="C236">
+        <v>193.26</v>
+      </c>
+      <c r="D236">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>57</v>
+      </c>
+      <c r="B237" t="s">
+        <v>16</v>
+      </c>
+      <c r="C237">
+        <v>272.93</v>
+      </c>
+      <c r="D237">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>57</v>
+      </c>
+      <c r="B238" t="s">
+        <v>17</v>
+      </c>
+      <c r="C238">
+        <v>288.12</v>
+      </c>
+      <c r="D238">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>57</v>
+      </c>
+      <c r="B239" t="s">
+        <v>18</v>
+      </c>
+      <c r="C239">
+        <v>137.49</v>
+      </c>
+      <c r="D239">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>57</v>
+      </c>
+      <c r="B240" t="s">
+        <v>19</v>
+      </c>
+      <c r="C240">
+        <v>40.1</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>57</v>
+      </c>
+      <c r="B241" t="s">
+        <v>20</v>
+      </c>
+      <c r="C241">
+        <v>128.58000000000001</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>57</v>
+      </c>
+      <c r="B242" t="s">
+        <v>21</v>
+      </c>
+      <c r="C242">
+        <v>85.6</v>
+      </c>
+      <c r="D242">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>57</v>
+      </c>
+      <c r="B243" t="s">
+        <v>22</v>
+      </c>
+      <c r="C243">
+        <v>132.94</v>
+      </c>
+      <c r="D243">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>57</v>
+      </c>
+      <c r="B244" t="s">
+        <v>23</v>
+      </c>
+      <c r="C244">
+        <v>281.07</v>
+      </c>
+      <c r="D244">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>57</v>
+      </c>
+      <c r="B245" t="s">
+        <v>24</v>
+      </c>
+      <c r="C245">
+        <v>57.95</v>
+      </c>
+      <c r="D245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>57</v>
+      </c>
+      <c r="B246" t="s">
+        <v>25</v>
+      </c>
+      <c r="C246">
+        <v>276.42</v>
+      </c>
+      <c r="D246">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>57</v>
+      </c>
+      <c r="B247" t="s">
+        <v>26</v>
+      </c>
+      <c r="C247">
+        <v>126.28</v>
+      </c>
+      <c r="D247">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>57</v>
+      </c>
+      <c r="B248" t="s">
+        <v>27</v>
+      </c>
+      <c r="C248">
+        <v>78.37</v>
+      </c>
+      <c r="D248">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>57</v>
+      </c>
+      <c r="B249" t="s">
+        <v>28</v>
+      </c>
+      <c r="C249">
+        <v>195.42</v>
+      </c>
+      <c r="D249">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>57</v>
+      </c>
+      <c r="B250" t="s">
+        <v>29</v>
+      </c>
+      <c r="C250">
+        <v>192.41</v>
+      </c>
+      <c r="D250">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>57</v>
+      </c>
+      <c r="B251" t="s">
+        <v>30</v>
+      </c>
+      <c r="C251">
+        <v>123.98</v>
+      </c>
+      <c r="D251">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>57</v>
+      </c>
+      <c r="B252" t="s">
+        <v>31</v>
+      </c>
+      <c r="C252">
+        <v>99.59</v>
+      </c>
+      <c r="D252">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>57</v>
+      </c>
+      <c r="B253" t="s">
+        <v>32</v>
+      </c>
+      <c r="C253">
+        <v>226.08</v>
+      </c>
+      <c r="D253">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>57</v>
+      </c>
+      <c r="B254" t="s">
+        <v>33</v>
+      </c>
+      <c r="C254">
+        <v>29.84</v>
+      </c>
+      <c r="D254">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>57</v>
+      </c>
+      <c r="B255" t="s">
+        <v>34</v>
+      </c>
+      <c r="C255">
+        <v>23.32</v>
+      </c>
+      <c r="D255">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>57</v>
+      </c>
+      <c r="B256" t="s">
+        <v>35</v>
+      </c>
+      <c r="C256">
+        <v>95.58</v>
+      </c>
+      <c r="D256">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>57</v>
+      </c>
+      <c r="B257" t="s">
+        <v>36</v>
+      </c>
+      <c r="C257">
+        <v>293.29000000000002</v>
+      </c>
+      <c r="D257">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>58</v>
+      </c>
+      <c r="B258" t="s">
+        <v>5</v>
+      </c>
+      <c r="C258">
+        <v>702.75</v>
+      </c>
+      <c r="D258">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>58</v>
+      </c>
+      <c r="B259" t="s">
+        <v>6</v>
+      </c>
+      <c r="C259">
+        <v>263.66000000000003</v>
+      </c>
+      <c r="D259">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>58</v>
+      </c>
+      <c r="B260" t="s">
+        <v>7</v>
+      </c>
+      <c r="C260">
+        <v>19.8</v>
+      </c>
+      <c r="D260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>58</v>
+      </c>
+      <c r="B261" t="s">
+        <v>8</v>
+      </c>
+      <c r="C261">
+        <v>236.82</v>
+      </c>
+      <c r="D261">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>58</v>
+      </c>
+      <c r="B262" t="s">
+        <v>9</v>
+      </c>
+      <c r="C262">
+        <v>33.1</v>
+      </c>
+      <c r="D262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>58</v>
+      </c>
+      <c r="B263" t="s">
+        <v>10</v>
+      </c>
+      <c r="C263">
+        <v>287.37</v>
+      </c>
+      <c r="D263">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>58</v>
+      </c>
+      <c r="B264" t="s">
+        <v>11</v>
+      </c>
+      <c r="C264">
+        <v>74.13</v>
+      </c>
+      <c r="D264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>58</v>
+      </c>
+      <c r="B265" t="s">
+        <v>12</v>
+      </c>
+      <c r="C265">
+        <v>39.57</v>
+      </c>
+      <c r="D265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>58</v>
+      </c>
+      <c r="B266" t="s">
+        <v>13</v>
+      </c>
+      <c r="C266">
+        <v>301.86</v>
+      </c>
+      <c r="D266">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>58</v>
+      </c>
+      <c r="B267" t="s">
+        <v>14</v>
+      </c>
+      <c r="C267">
+        <v>118.1</v>
+      </c>
+      <c r="D267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>58</v>
+      </c>
+      <c r="B268" t="s">
+        <v>15</v>
+      </c>
+      <c r="C268">
+        <v>199.49</v>
+      </c>
+      <c r="D268">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>58</v>
+      </c>
+      <c r="B269" t="s">
+        <v>16</v>
+      </c>
+      <c r="C269">
+        <v>279.17</v>
+      </c>
+      <c r="D269">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>58</v>
+      </c>
+      <c r="B270" t="s">
+        <v>17</v>
+      </c>
+      <c r="C270">
+        <v>291.04000000000002</v>
+      </c>
+      <c r="D270">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>58</v>
+      </c>
+      <c r="B271" t="s">
+        <v>18</v>
+      </c>
+      <c r="C271">
+        <v>144.58000000000001</v>
+      </c>
+      <c r="D271">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>58</v>
+      </c>
+      <c r="B272" t="s">
+        <v>19</v>
+      </c>
+      <c r="C272">
+        <v>40.1</v>
+      </c>
+      <c r="D272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>58</v>
+      </c>
+      <c r="B273" t="s">
+        <v>20</v>
+      </c>
+      <c r="C273">
+        <v>128.58000000000001</v>
+      </c>
+      <c r="D273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>58</v>
+      </c>
+      <c r="B274" t="s">
+        <v>21</v>
+      </c>
+      <c r="C274">
+        <v>86.61</v>
+      </c>
+      <c r="D274">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>58</v>
+      </c>
+      <c r="B275" t="s">
+        <v>22</v>
+      </c>
+      <c r="C275">
+        <v>133.24</v>
+      </c>
+      <c r="D275">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>58</v>
+      </c>
+      <c r="B276" t="s">
+        <v>23</v>
+      </c>
+      <c r="C276">
+        <v>283.24</v>
+      </c>
+      <c r="D276">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>58</v>
+      </c>
+      <c r="B277" t="s">
+        <v>24</v>
+      </c>
+      <c r="C277">
+        <v>59.74</v>
+      </c>
+      <c r="D277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>58</v>
+      </c>
+      <c r="B278" t="s">
+        <v>25</v>
+      </c>
+      <c r="C278">
+        <v>278.14999999999998</v>
+      </c>
+      <c r="D278">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>58</v>
+      </c>
+      <c r="B279" t="s">
+        <v>26</v>
+      </c>
+      <c r="C279">
+        <v>126.28</v>
+      </c>
+      <c r="D279">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>58</v>
+      </c>
+      <c r="B280" t="s">
+        <v>27</v>
+      </c>
+      <c r="C280">
+        <v>79.03</v>
+      </c>
+      <c r="D280">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>58</v>
+      </c>
+      <c r="B281" t="s">
+        <v>28</v>
+      </c>
+      <c r="C281">
+        <v>197.4</v>
+      </c>
+      <c r="D281">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>58</v>
+      </c>
+      <c r="B282" t="s">
+        <v>29</v>
+      </c>
+      <c r="C282">
+        <v>195.28</v>
+      </c>
+      <c r="D282">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>58</v>
+      </c>
+      <c r="B283" t="s">
+        <v>30</v>
+      </c>
+      <c r="C283">
+        <v>123.98</v>
+      </c>
+      <c r="D283">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>58</v>
+      </c>
+      <c r="B284" t="s">
+        <v>31</v>
+      </c>
+      <c r="C284">
+        <v>100.16</v>
+      </c>
+      <c r="D284">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>58</v>
+      </c>
+      <c r="B285" t="s">
+        <v>32</v>
+      </c>
+      <c r="C285">
+        <v>226.08</v>
+      </c>
+      <c r="D285">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>58</v>
+      </c>
+      <c r="B286" t="s">
+        <v>33</v>
+      </c>
+      <c r="C286">
+        <v>29.84</v>
+      </c>
+      <c r="D286">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>58</v>
+      </c>
+      <c r="B287" t="s">
+        <v>34</v>
+      </c>
+      <c r="C287">
+        <v>24.49</v>
+      </c>
+      <c r="D287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>58</v>
+      </c>
+      <c r="B288" t="s">
+        <v>35</v>
+      </c>
+      <c r="C288">
+        <v>95.58</v>
+      </c>
+      <c r="D288">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>58</v>
+      </c>
+      <c r="B289" t="s">
+        <v>36</v>
+      </c>
+      <c r="C289">
+        <v>299.04000000000002</v>
+      </c>
+      <c r="D289">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3288,7 +4641,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,15 +4732,33 @@
       <c r="A8" s="2">
         <v>44004</v>
       </c>
+      <c r="B8">
+        <v>1970</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44005</v>
       </c>
+      <c r="B9">
+        <v>2973</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44006</v>
+      </c>
+      <c r="B10">
+        <v>2251</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Delete files no longer needed
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C09A2-FB16-4EB2-923B-32F713FFF880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F6F285-0A71-453D-B25C-7922199C2DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="195" windowWidth="9900" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
+    <workbookView xWindow="765" yWindow="285" windowWidth="9900" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fallecido_Recuperado" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Fallecidos %</t>
-  </si>
-  <si>
-    <t>24/6/2020</t>
   </si>
   <si>
     <t>Casos Confirmados</t>
@@ -551,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,13 +567,13 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -745,6 +742,62 @@
       </c>
       <c r="D13">
         <v>14216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B14">
+        <v>28631</v>
+      </c>
+      <c r="C14">
+        <v>691</v>
+      </c>
+      <c r="D14">
+        <v>16006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B15">
+        <v>33387</v>
+      </c>
+      <c r="C15">
+        <v>754</v>
+      </c>
+      <c r="D15">
+        <v>17904</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B16">
+        <v>39588</v>
+      </c>
+      <c r="C16">
+        <v>829</v>
+      </c>
+      <c r="D16">
+        <v>20056</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B17">
+        <v>47671</v>
+      </c>
+      <c r="C17">
+        <v>929</v>
+      </c>
+      <c r="D17">
+        <v>23459</v>
       </c>
     </row>
   </sheetData>
@@ -754,10 +807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D449"/>
+  <dimension ref="A1:D513"/>
   <sheetViews>
-    <sheetView topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="A387" sqref="A386:A417"/>
+    <sheetView topLeftCell="A486" workbookViewId="0">
+      <selection activeCell="D514" sqref="D514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6511,451 +6564,1347 @@
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A418" t="s">
-        <v>48</v>
+      <c r="A418" s="2">
+        <v>44012</v>
       </c>
       <c r="B418" t="s">
         <v>4</v>
       </c>
       <c r="C418">
-        <v>702.75</v>
+        <v>831.11</v>
       </c>
       <c r="D418">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A419" t="s">
-        <v>48</v>
+      <c r="A419" s="2">
+        <v>44012</v>
       </c>
       <c r="B419" t="s">
         <v>5</v>
       </c>
       <c r="C419">
-        <v>263.66000000000003</v>
+        <v>289.31</v>
       </c>
       <c r="D419">
         <v>10</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A420" t="s">
-        <v>48</v>
+      <c r="A420" s="2">
+        <v>44012</v>
       </c>
       <c r="B420" t="s">
         <v>6</v>
       </c>
       <c r="C420">
-        <v>19.8</v>
+        <v>27.72</v>
       </c>
       <c r="D420">
         <v>1</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A421" t="s">
-        <v>48</v>
+      <c r="A421" s="2">
+        <v>44012</v>
       </c>
       <c r="B421" t="s">
         <v>7</v>
       </c>
       <c r="C421">
-        <v>236.82</v>
+        <v>305.52999999999997</v>
       </c>
       <c r="D421">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A422" t="s">
-        <v>48</v>
+      <c r="A422" s="2">
+        <v>44012</v>
       </c>
       <c r="B422" t="s">
         <v>8</v>
       </c>
       <c r="C422">
-        <v>33.1</v>
+        <v>49.65</v>
       </c>
       <c r="D422">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A423" t="s">
-        <v>48</v>
+      <c r="A423" s="2">
+        <v>44012</v>
       </c>
       <c r="B423" t="s">
         <v>9</v>
       </c>
       <c r="C423">
-        <v>287.37</v>
+        <v>300.42</v>
       </c>
       <c r="D423">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A424" t="s">
-        <v>48</v>
+      <c r="A424" s="2">
+        <v>44012</v>
       </c>
       <c r="B424" t="s">
         <v>10</v>
       </c>
       <c r="C424">
-        <v>74.13</v>
+        <v>130.91</v>
       </c>
       <c r="D424">
         <v>1</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A425" t="s">
-        <v>48</v>
+      <c r="A425" s="2">
+        <v>44012</v>
       </c>
       <c r="B425" t="s">
         <v>11</v>
       </c>
       <c r="C425">
-        <v>39.57</v>
+        <v>49.19</v>
       </c>
       <c r="D425">
         <v>0</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A426" t="s">
-        <v>48</v>
+      <c r="A426" s="2">
+        <v>44012</v>
       </c>
       <c r="B426" t="s">
         <v>12</v>
       </c>
       <c r="C426">
-        <v>301.86</v>
+        <v>313.95</v>
       </c>
       <c r="D426">
         <v>14</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A427" t="s">
-        <v>48</v>
+      <c r="A427" s="2">
+        <v>44012</v>
       </c>
       <c r="B427" t="s">
         <v>13</v>
       </c>
       <c r="C427">
-        <v>118.1</v>
+        <v>147.19999999999999</v>
       </c>
       <c r="D427">
         <v>1</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A428" t="s">
-        <v>48</v>
+      <c r="A428" s="2">
+        <v>44012</v>
       </c>
       <c r="B428" t="s">
         <v>14</v>
       </c>
       <c r="C428">
-        <v>199.49</v>
+        <v>230.61</v>
       </c>
       <c r="D428">
         <v>2</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A429" t="s">
-        <v>48</v>
+      <c r="A429" s="2">
+        <v>44012</v>
       </c>
       <c r="B429" t="s">
         <v>15</v>
       </c>
       <c r="C429">
-        <v>279.17</v>
+        <v>317.32</v>
       </c>
       <c r="D429">
         <v>10</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A430" t="s">
-        <v>48</v>
+      <c r="A430" s="2">
+        <v>44012</v>
       </c>
       <c r="B430" t="s">
         <v>16</v>
       </c>
       <c r="C430">
-        <v>291.04000000000002</v>
+        <v>319.24</v>
       </c>
       <c r="D430">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A431" t="s">
-        <v>48</v>
+      <c r="A431" s="2">
+        <v>44012</v>
       </c>
       <c r="B431" t="s">
         <v>17</v>
       </c>
       <c r="C431">
-        <v>144.58000000000001</v>
+        <v>159.46</v>
       </c>
       <c r="D431">
         <v>4</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A432" t="s">
-        <v>48</v>
+      <c r="A432" s="2">
+        <v>44012</v>
       </c>
       <c r="B432" t="s">
         <v>18</v>
       </c>
       <c r="C432">
-        <v>40.1</v>
+        <v>51.19</v>
       </c>
       <c r="D432">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A433" t="s">
-        <v>48</v>
+      <c r="A433" s="2">
+        <v>44012</v>
       </c>
       <c r="B433" t="s">
         <v>19</v>
       </c>
       <c r="C433">
-        <v>128.58000000000001</v>
+        <v>162.87</v>
       </c>
       <c r="D433">
         <v>0</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A434" t="s">
-        <v>48</v>
+      <c r="A434" s="2">
+        <v>44012</v>
       </c>
       <c r="B434" t="s">
         <v>20</v>
       </c>
       <c r="C434">
-        <v>86.61</v>
+        <v>104.85</v>
       </c>
       <c r="D434">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A435" t="s">
-        <v>48</v>
+      <c r="A435" s="2">
+        <v>44012</v>
       </c>
       <c r="B435" t="s">
         <v>21</v>
       </c>
       <c r="C435">
-        <v>133.24</v>
+        <v>157.25</v>
       </c>
       <c r="D435">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A436" t="s">
-        <v>48</v>
+      <c r="A436" s="2">
+        <v>44012</v>
       </c>
       <c r="B436" t="s">
         <v>22</v>
       </c>
       <c r="C436">
-        <v>283.24</v>
+        <v>293.01</v>
       </c>
       <c r="D436">
         <v>18</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A437" t="s">
-        <v>48</v>
+      <c r="A437" s="2">
+        <v>44012</v>
       </c>
       <c r="B437" t="s">
         <v>23</v>
       </c>
       <c r="C437">
-        <v>59.74</v>
+        <v>62.41</v>
       </c>
       <c r="D437">
         <v>1</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A438" t="s">
-        <v>48</v>
+      <c r="A438" s="2">
+        <v>44012</v>
       </c>
       <c r="B438" t="s">
         <v>24</v>
       </c>
       <c r="C438">
-        <v>278.14999999999998</v>
+        <v>301.83999999999997</v>
       </c>
       <c r="D438">
         <v>31</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A439" t="s">
-        <v>48</v>
+      <c r="A439" s="2">
+        <v>44012</v>
       </c>
       <c r="B439" t="s">
         <v>25</v>
       </c>
       <c r="C439">
-        <v>126.28</v>
+        <v>158.75</v>
       </c>
       <c r="D439">
         <v>8</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A440" t="s">
-        <v>48</v>
+      <c r="A440" s="2">
+        <v>44012</v>
       </c>
       <c r="B440" t="s">
         <v>26</v>
       </c>
       <c r="C440">
-        <v>79.03</v>
+        <v>97.72</v>
       </c>
       <c r="D440">
         <v>14</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A441" t="s">
-        <v>48</v>
+      <c r="A441" s="2">
+        <v>44012</v>
       </c>
       <c r="B441" t="s">
         <v>27</v>
       </c>
       <c r="C441">
-        <v>197.4</v>
+        <v>219.11</v>
       </c>
       <c r="D441">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A442" t="s">
-        <v>48</v>
+      <c r="A442" s="2">
+        <v>44012</v>
       </c>
       <c r="B442" t="s">
         <v>28</v>
       </c>
       <c r="C442">
-        <v>195.28</v>
+        <v>229.15</v>
       </c>
       <c r="D442">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A443" t="s">
-        <v>48</v>
+      <c r="A443" s="2">
+        <v>44012</v>
       </c>
       <c r="B443" t="s">
         <v>29</v>
       </c>
       <c r="C443">
-        <v>123.98</v>
+        <v>144.94</v>
       </c>
       <c r="D443">
         <v>4</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A444" t="s">
-        <v>48</v>
+      <c r="A444" s="2">
+        <v>44012</v>
       </c>
       <c r="B444" t="s">
         <v>30</v>
       </c>
       <c r="C444">
-        <v>100.16</v>
+        <v>132.97999999999999</v>
       </c>
       <c r="D444">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A445" t="s">
-        <v>48</v>
+      <c r="A445" s="2">
+        <v>44012</v>
       </c>
       <c r="B445" t="s">
         <v>31</v>
       </c>
       <c r="C445">
-        <v>226.08</v>
+        <v>245.01</v>
       </c>
       <c r="D445">
         <v>7</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A446" t="s">
-        <v>48</v>
+      <c r="A446" s="2">
+        <v>44012</v>
       </c>
       <c r="B446" t="s">
         <v>32</v>
       </c>
       <c r="C446">
-        <v>29.84</v>
+        <v>34.03</v>
       </c>
       <c r="D446">
         <v>7</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A447" t="s">
-        <v>48</v>
+      <c r="A447" s="2">
+        <v>44012</v>
       </c>
       <c r="B447" t="s">
         <v>33</v>
       </c>
       <c r="C447">
-        <v>24.49</v>
+        <v>38.479999999999997</v>
       </c>
       <c r="D447">
         <v>2</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A448" t="s">
-        <v>48</v>
+      <c r="A448" s="2">
+        <v>44012</v>
       </c>
       <c r="B448" t="s">
         <v>34</v>
       </c>
       <c r="C448">
-        <v>95.58</v>
+        <v>136.02000000000001</v>
       </c>
       <c r="D448">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A449" t="s">
-        <v>48</v>
+      <c r="A449" s="2">
+        <v>44012</v>
       </c>
       <c r="B449" t="s">
         <v>35</v>
       </c>
       <c r="C449">
-        <v>299.04000000000002</v>
+        <v>339.23</v>
       </c>
       <c r="D449">
-        <v>153</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A450" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B450" t="s">
+        <v>4</v>
+      </c>
+      <c r="C450">
+        <v>1035.96</v>
+      </c>
+      <c r="D450">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B451" t="s">
+        <v>5</v>
+      </c>
+      <c r="C451">
+        <v>340.15</v>
+      </c>
+      <c r="D451">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B452" t="s">
+        <v>6</v>
+      </c>
+      <c r="C452">
+        <v>43.56</v>
+      </c>
+      <c r="D452">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A453" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B453" t="s">
+        <v>7</v>
+      </c>
+      <c r="C453">
+        <v>342.01</v>
+      </c>
+      <c r="D453">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A454" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B454" t="s">
+        <v>8</v>
+      </c>
+      <c r="C454">
+        <v>75.23</v>
+      </c>
+      <c r="D454">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A455" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B455" t="s">
+        <v>9</v>
+      </c>
+      <c r="C455">
+        <v>320.49</v>
+      </c>
+      <c r="D455">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A456" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B456" t="s">
+        <v>10</v>
+      </c>
+      <c r="C456">
+        <v>171.92</v>
+      </c>
+      <c r="D456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A457" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B457" t="s">
+        <v>11</v>
+      </c>
+      <c r="C457">
+        <v>66.3</v>
+      </c>
+      <c r="D457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A458" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B458" t="s">
+        <v>12</v>
+      </c>
+      <c r="C458">
+        <v>349.39</v>
+      </c>
+      <c r="D458">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A459" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B459" t="s">
+        <v>13</v>
+      </c>
+      <c r="C459">
+        <v>219.09</v>
+      </c>
+      <c r="D459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A460" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B460" t="s">
+        <v>14</v>
+      </c>
+      <c r="C460">
+        <v>288.62</v>
+      </c>
+      <c r="D460">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A461" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B461" t="s">
+        <v>15</v>
+      </c>
+      <c r="C461">
+        <v>362.81</v>
+      </c>
+      <c r="D461">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A462" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B462" t="s">
+        <v>16</v>
+      </c>
+      <c r="C462">
+        <v>362.52</v>
+      </c>
+      <c r="D462">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A463" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B463" t="s">
+        <v>17</v>
+      </c>
+      <c r="C463">
+        <v>186.4</v>
+      </c>
+      <c r="D463">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A464" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B464" t="s">
+        <v>18</v>
+      </c>
+      <c r="C464">
+        <v>59.72</v>
+      </c>
+      <c r="D464">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A465" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B465" t="s">
+        <v>19</v>
+      </c>
+      <c r="C465">
+        <v>274.31</v>
+      </c>
+      <c r="D465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A466" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B466" t="s">
+        <v>20</v>
+      </c>
+      <c r="C466">
+        <v>127.13</v>
+      </c>
+      <c r="D466">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A467" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B467" t="s">
+        <v>21</v>
+      </c>
+      <c r="C467">
+        <v>184.86</v>
+      </c>
+      <c r="D467">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A468" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B468" t="s">
+        <v>22</v>
+      </c>
+      <c r="C468">
+        <v>312.54000000000002</v>
+      </c>
+      <c r="D468">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A469" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B469" t="s">
+        <v>23</v>
+      </c>
+      <c r="C469">
+        <v>77.569999999999993</v>
+      </c>
+      <c r="D469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A470" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B470" t="s">
+        <v>24</v>
+      </c>
+      <c r="C470">
+        <v>339.8</v>
+      </c>
+      <c r="D470">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B471" t="s">
+        <v>25</v>
+      </c>
+      <c r="C471">
+        <v>211.51</v>
+      </c>
+      <c r="D471">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B472" t="s">
+        <v>26</v>
+      </c>
+      <c r="C472">
+        <v>124.6</v>
+      </c>
+      <c r="D472">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B473" t="s">
+        <v>27</v>
+      </c>
+      <c r="C473">
+        <v>255.96</v>
+      </c>
+      <c r="D473">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B474" t="s">
+        <v>28</v>
+      </c>
+      <c r="C474">
+        <v>293.35000000000002</v>
+      </c>
+      <c r="D474">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A475" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B475" t="s">
+        <v>29</v>
+      </c>
+      <c r="C475">
+        <v>151.91999999999999</v>
+      </c>
+      <c r="D475">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A476" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B476" t="s">
+        <v>30</v>
+      </c>
+      <c r="C476">
+        <v>139.77000000000001</v>
+      </c>
+      <c r="D476">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A477" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B477" t="s">
+        <v>31</v>
+      </c>
+      <c r="C477">
+        <v>270.83</v>
+      </c>
+      <c r="D477">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B478" t="s">
+        <v>32</v>
+      </c>
+      <c r="C478">
+        <v>39.78</v>
+      </c>
+      <c r="D478">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A479" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B479" t="s">
+        <v>33</v>
+      </c>
+      <c r="C479">
+        <v>51.3</v>
+      </c>
+      <c r="D479">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A480" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B480" t="s">
+        <v>34</v>
+      </c>
+      <c r="C480">
+        <v>185.64</v>
+      </c>
+      <c r="D480">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A481" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B481" t="s">
+        <v>35</v>
+      </c>
+      <c r="C481">
+        <v>390.43</v>
+      </c>
+      <c r="D481">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A482" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B482" t="s">
+        <v>4</v>
+      </c>
+      <c r="C482">
+        <v>1257.3</v>
+      </c>
+      <c r="D482">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A483" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B483" t="s">
+        <v>5</v>
+      </c>
+      <c r="C483">
+        <v>404.04</v>
+      </c>
+      <c r="D483">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A484" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B484" t="s">
+        <v>6</v>
+      </c>
+      <c r="C484">
+        <v>45.54</v>
+      </c>
+      <c r="D484">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A485" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B485" t="s">
+        <v>7</v>
+      </c>
+      <c r="C485">
+        <v>357.34</v>
+      </c>
+      <c r="D485">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A486" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B486" t="s">
+        <v>8</v>
+      </c>
+      <c r="C486">
+        <v>102.31</v>
+      </c>
+      <c r="D486">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A487" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B487" t="s">
+        <v>9</v>
+      </c>
+      <c r="C487">
+        <v>361.64</v>
+      </c>
+      <c r="D487">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A488" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B488" t="s">
+        <v>10</v>
+      </c>
+      <c r="C488">
+        <v>209.77</v>
+      </c>
+      <c r="D488">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A489" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B489" t="s">
+        <v>11</v>
+      </c>
+      <c r="C489">
+        <v>112.29</v>
+      </c>
+      <c r="D489">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A490" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B490" t="s">
+        <v>12</v>
+      </c>
+      <c r="C490">
+        <v>411.93</v>
+      </c>
+      <c r="D490">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A491" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B491" t="s">
+        <v>13</v>
+      </c>
+      <c r="C491">
+        <v>220.8</v>
+      </c>
+      <c r="D491">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A492" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B492" t="s">
+        <v>14</v>
+      </c>
+      <c r="C492">
+        <v>398.13</v>
+      </c>
+      <c r="D492">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A493" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B493" t="s">
+        <v>15</v>
+      </c>
+      <c r="C493">
+        <v>420.77</v>
+      </c>
+      <c r="D493">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A494" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B494" t="s">
+        <v>16</v>
+      </c>
+      <c r="C494">
+        <v>414.79</v>
+      </c>
+      <c r="D494">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A495" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B495" t="s">
+        <v>17</v>
+      </c>
+      <c r="C495">
+        <v>236.01</v>
+      </c>
+      <c r="D495">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A496" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B496" t="s">
+        <v>18</v>
+      </c>
+      <c r="C496">
+        <v>73.37</v>
+      </c>
+      <c r="D496">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A497" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B497" t="s">
+        <v>19</v>
+      </c>
+      <c r="C497">
+        <v>320.02999999999997</v>
+      </c>
+      <c r="D497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A498" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B498" t="s">
+        <v>20</v>
+      </c>
+      <c r="C498">
+        <v>166.13</v>
+      </c>
+      <c r="D498">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A499" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B499" t="s">
+        <v>21</v>
+      </c>
+      <c r="C499">
+        <v>217.87</v>
+      </c>
+      <c r="D499">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A500" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B500" t="s">
+        <v>22</v>
+      </c>
+      <c r="C500">
+        <v>333.16</v>
+      </c>
+      <c r="D500">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A501" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B501" t="s">
+        <v>23</v>
+      </c>
+      <c r="C501">
+        <v>171.18</v>
+      </c>
+      <c r="D501">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A502" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B502" t="s">
+        <v>24</v>
+      </c>
+      <c r="C502">
+        <v>366.47</v>
+      </c>
+      <c r="D502">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A503" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B503" t="s">
+        <v>25</v>
+      </c>
+      <c r="C503">
+        <v>289.98</v>
+      </c>
+      <c r="D503">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A504" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B504" t="s">
+        <v>26</v>
+      </c>
+      <c r="C504">
+        <v>169.86</v>
+      </c>
+      <c r="D504">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A505" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B505" t="s">
+        <v>27</v>
+      </c>
+      <c r="C505">
+        <v>353.54</v>
+      </c>
+      <c r="D505">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A506" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B506" t="s">
+        <v>28</v>
+      </c>
+      <c r="C506">
+        <v>379.27</v>
+      </c>
+      <c r="D506">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A507" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B507" t="s">
+        <v>29</v>
+      </c>
+      <c r="C507">
+        <v>195.58</v>
+      </c>
+      <c r="D507">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A508" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B508" t="s">
+        <v>30</v>
+      </c>
+      <c r="C508">
+        <v>142.6</v>
+      </c>
+      <c r="D508">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A509" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B509" t="s">
+        <v>31</v>
+      </c>
+      <c r="C509">
+        <v>298.77</v>
+      </c>
+      <c r="D509">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A510" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B510" t="s">
+        <v>32</v>
+      </c>
+      <c r="C510">
+        <v>52.87</v>
+      </c>
+      <c r="D510">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A511" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B511" t="s">
+        <v>33</v>
+      </c>
+      <c r="C511">
+        <v>66.459999999999994</v>
+      </c>
+      <c r="D511">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A512" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B512" t="s">
+        <v>34</v>
+      </c>
+      <c r="C512">
+        <v>191.16</v>
+      </c>
+      <c r="D512">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A513" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B513" t="s">
+        <v>35</v>
+      </c>
+      <c r="C513">
+        <v>444.25</v>
+      </c>
+      <c r="D513">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -6967,10 +7916,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422A3AD-6985-4C77-AE63-323FE7C4AE0C}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6995,7 +7944,7 @@
         <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7797,6 +8746,384 @@
       </c>
       <c r="D64">
         <v>63.05</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B65" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65">
+        <v>0.4</v>
+      </c>
+      <c r="D65">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66">
+        <v>1.5</v>
+      </c>
+      <c r="D66">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67">
+        <v>1.9</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68">
+        <v>4.8</v>
+      </c>
+      <c r="D68">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B69" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="D69">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B70" t="s">
+        <v>39</v>
+      </c>
+      <c r="C70">
+        <v>22.45</v>
+      </c>
+      <c r="D70">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71">
+        <v>17.5</v>
+      </c>
+      <c r="D71">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72">
+        <v>13.85</v>
+      </c>
+      <c r="D72">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73">
+        <v>15.05</v>
+      </c>
+      <c r="D73">
+        <v>63.55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B74" t="s">
+        <v>37</v>
+      </c>
+      <c r="C74">
+        <v>0.45</v>
+      </c>
+      <c r="D74">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C75">
+        <v>1.55</v>
+      </c>
+      <c r="D75">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76">
+        <v>1.9</v>
+      </c>
+      <c r="D76">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77">
+        <v>4.75</v>
+      </c>
+      <c r="D77">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B78" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D78">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79">
+        <v>22.6</v>
+      </c>
+      <c r="D79">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80">
+        <v>17.45</v>
+      </c>
+      <c r="D80">
+        <v>8.5500000000000007</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B81" t="s">
+        <v>41</v>
+      </c>
+      <c r="C81">
+        <v>13.7</v>
+      </c>
+      <c r="D81">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B82" t="s">
+        <v>42</v>
+      </c>
+      <c r="C82">
+        <v>14.8</v>
+      </c>
+      <c r="D82">
+        <v>63.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B83" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83">
+        <v>0.45</v>
+      </c>
+      <c r="D83">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C84">
+        <v>1.65</v>
+      </c>
+      <c r="D84">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85">
+        <v>1.9</v>
+      </c>
+      <c r="D85">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C86">
+        <v>4.7</v>
+      </c>
+      <c r="D86">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B87" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87">
+        <v>19.45</v>
+      </c>
+      <c r="D87">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88">
+        <v>22.8</v>
+      </c>
+      <c r="D88">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89">
+        <v>17.5</v>
+      </c>
+      <c r="D89">
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B90" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90">
+        <v>13.55</v>
+      </c>
+      <c r="D90">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B91" t="s">
+        <v>42</v>
+      </c>
+      <c r="C91">
+        <v>14.7</v>
+      </c>
+      <c r="D91">
+        <v>64.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Several more weeks of data
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD4E651-7FE4-48A6-8469-BC9D2EBA370D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C3CA8C-C451-4EFA-8A99-4AA1E85CEAED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="150" windowWidth="9540" windowHeight="12435" firstSheet="2" activeTab="2" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
+    <workbookView xWindow="765" yWindow="210" windowWidth="9540" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fallecido_Recuperado" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,6 +850,62 @@
         <v>47095</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B22">
+        <v>88127</v>
+      </c>
+      <c r="C22">
+        <v>1501</v>
+      </c>
+      <c r="D22">
+        <v>56760</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B23">
+        <v>92557</v>
+      </c>
+      <c r="C23">
+        <v>1613</v>
+      </c>
+      <c r="D23">
+        <v>63478</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B24">
+        <v>95627</v>
+      </c>
+      <c r="C24">
+        <v>1765</v>
+      </c>
+      <c r="D24">
+        <v>69519</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B25">
+        <v>100131</v>
+      </c>
+      <c r="C25">
+        <v>1889</v>
+      </c>
+      <c r="D25">
+        <v>73795</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -857,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D641"/>
+  <dimension ref="A1:D769"/>
   <sheetViews>
-    <sheetView topLeftCell="A615" workbookViewId="0">
-      <selection activeCell="B642" sqref="B642"/>
+    <sheetView tabSelected="1" topLeftCell="A744" workbookViewId="0">
+      <selection activeCell="D770" sqref="D770"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9749,6 +9805,1798 @@
         <v>336</v>
       </c>
     </row>
+    <row r="642" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A642" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B642" t="s">
+        <v>4</v>
+      </c>
+      <c r="C642">
+        <v>2406.09</v>
+      </c>
+      <c r="D642">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="643" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A643" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B643" t="s">
+        <v>5</v>
+      </c>
+      <c r="C643">
+        <v>709.99</v>
+      </c>
+      <c r="D643">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="644" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A644" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B644" t="s">
+        <v>6</v>
+      </c>
+      <c r="C644">
+        <v>327.71</v>
+      </c>
+      <c r="D644">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="645" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A645" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B645" t="s">
+        <v>7</v>
+      </c>
+      <c r="C645">
+        <v>706.75</v>
+      </c>
+      <c r="D645">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="646" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A646" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B646" t="s">
+        <v>8</v>
+      </c>
+      <c r="C646">
+        <v>246.74</v>
+      </c>
+      <c r="D646">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="647" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A647" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B647" t="s">
+        <v>9</v>
+      </c>
+      <c r="C647">
+        <v>679.8</v>
+      </c>
+      <c r="D647">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A648" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B648" t="s">
+        <v>10</v>
+      </c>
+      <c r="C648">
+        <v>328.07</v>
+      </c>
+      <c r="D648">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="649" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A649" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B649" t="s">
+        <v>11</v>
+      </c>
+      <c r="C649">
+        <v>343.29</v>
+      </c>
+      <c r="D649">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="650" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A650" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B650" t="s">
+        <v>12</v>
+      </c>
+      <c r="C650">
+        <v>611.65</v>
+      </c>
+      <c r="D650">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A651" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B651" t="s">
+        <v>13</v>
+      </c>
+      <c r="C651">
+        <v>332.06</v>
+      </c>
+      <c r="D651">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A652" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B652" t="s">
+        <v>14</v>
+      </c>
+      <c r="C652">
+        <v>883.12</v>
+      </c>
+      <c r="D652">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A653" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B653" t="s">
+        <v>15</v>
+      </c>
+      <c r="C653">
+        <v>692.96</v>
+      </c>
+      <c r="D653">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A654" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B654" t="s">
+        <v>16</v>
+      </c>
+      <c r="C654">
+        <v>753.48</v>
+      </c>
+      <c r="D654">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A655" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B655" t="s">
+        <v>17</v>
+      </c>
+      <c r="C655">
+        <v>712.28</v>
+      </c>
+      <c r="D655">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A656" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B656" t="s">
+        <v>18</v>
+      </c>
+      <c r="C656">
+        <v>187.68</v>
+      </c>
+      <c r="D656">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A657" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B657" t="s">
+        <v>19</v>
+      </c>
+      <c r="C657">
+        <v>1231.53</v>
+      </c>
+      <c r="D657">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="658" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A658" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B658" t="s">
+        <v>20</v>
+      </c>
+      <c r="C658">
+        <v>445.72</v>
+      </c>
+      <c r="D658">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="659" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A659" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B659" t="s">
+        <v>21</v>
+      </c>
+      <c r="C659">
+        <v>469.06</v>
+      </c>
+      <c r="D659">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A660" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B660" t="s">
+        <v>22</v>
+      </c>
+      <c r="C660">
+        <v>417.81</v>
+      </c>
+      <c r="D660">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="661" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A661" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B661" t="s">
+        <v>23</v>
+      </c>
+      <c r="C661">
+        <v>214.87</v>
+      </c>
+      <c r="D661">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A662" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B662" t="s">
+        <v>24</v>
+      </c>
+      <c r="C662">
+        <v>527.9</v>
+      </c>
+      <c r="D662">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="663" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A663" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B663" t="s">
+        <v>25</v>
+      </c>
+      <c r="C663">
+        <v>555.16</v>
+      </c>
+      <c r="D663">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="664" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A664" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B664" t="s">
+        <v>26</v>
+      </c>
+      <c r="C664">
+        <v>410.87</v>
+      </c>
+      <c r="D664">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="665" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A665" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B665" t="s">
+        <v>27</v>
+      </c>
+      <c r="C665">
+        <v>800.12</v>
+      </c>
+      <c r="D665">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="666" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A666" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B666" t="s">
+        <v>28</v>
+      </c>
+      <c r="C666">
+        <v>886.36</v>
+      </c>
+      <c r="D666">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="667" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A667" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B667" t="s">
+        <v>29</v>
+      </c>
+      <c r="C667">
+        <v>640.87</v>
+      </c>
+      <c r="D667">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="668" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A668" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B668" t="s">
+        <v>30</v>
+      </c>
+      <c r="C668">
+        <v>232.57</v>
+      </c>
+      <c r="D668">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A669" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B669" t="s">
+        <v>31</v>
+      </c>
+      <c r="C669">
+        <v>530.76</v>
+      </c>
+      <c r="D669">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="670" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A670" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B670" t="s">
+        <v>32</v>
+      </c>
+      <c r="C670">
+        <v>104.17</v>
+      </c>
+      <c r="D670">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="671" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A671" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B671" t="s">
+        <v>33</v>
+      </c>
+      <c r="C671">
+        <v>171.4</v>
+      </c>
+      <c r="D671">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="672" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A672" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B672" t="s">
+        <v>34</v>
+      </c>
+      <c r="C672">
+        <v>595.53</v>
+      </c>
+      <c r="D672">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="673" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A673" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B673" t="s">
+        <v>35</v>
+      </c>
+      <c r="C673">
+        <v>661.53</v>
+      </c>
+      <c r="D673">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="674" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A674" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B674" t="s">
+        <v>4</v>
+      </c>
+      <c r="C674">
+        <v>2531.67</v>
+      </c>
+      <c r="D674">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="675" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A675" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B675" t="s">
+        <v>5</v>
+      </c>
+      <c r="C675">
+        <v>732.49</v>
+      </c>
+      <c r="D675">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="676" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A676" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B676" t="s">
+        <v>6</v>
+      </c>
+      <c r="C676">
+        <v>392.06</v>
+      </c>
+      <c r="D676">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="677" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A677" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B677" t="s">
+        <v>7</v>
+      </c>
+      <c r="C677">
+        <v>723.13</v>
+      </c>
+      <c r="D677">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="678" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A678" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B678" t="s">
+        <v>8</v>
+      </c>
+      <c r="C678">
+        <v>246.74</v>
+      </c>
+      <c r="D678">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="679" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A679" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B679" t="s">
+        <v>9</v>
+      </c>
+      <c r="C679">
+        <v>732.65</v>
+      </c>
+      <c r="D679">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="680" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A680" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B680" t="s">
+        <v>10</v>
+      </c>
+      <c r="C680">
+        <v>329.64</v>
+      </c>
+      <c r="D680">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="681" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A681" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B681" t="s">
+        <v>11</v>
+      </c>
+      <c r="C681">
+        <v>347.65</v>
+      </c>
+      <c r="D681">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="682" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A682" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B682" t="s">
+        <v>12</v>
+      </c>
+      <c r="C682">
+        <v>620.4</v>
+      </c>
+      <c r="D682">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="683" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A683" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B683" t="s">
+        <v>13</v>
+      </c>
+      <c r="C683">
+        <v>333.77</v>
+      </c>
+      <c r="D683">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="684" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A684" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B684" t="s">
+        <v>14</v>
+      </c>
+      <c r="C684">
+        <v>931.51</v>
+      </c>
+      <c r="D684">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="685" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A685" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B685" t="s">
+        <v>15</v>
+      </c>
+      <c r="C685">
+        <v>736.99</v>
+      </c>
+      <c r="D685">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="686" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A686" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B686" t="s">
+        <v>16</v>
+      </c>
+      <c r="C686">
+        <v>794.82</v>
+      </c>
+      <c r="D686">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="687" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A687" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B687" t="s">
+        <v>17</v>
+      </c>
+      <c r="C687">
+        <v>747</v>
+      </c>
+      <c r="D687">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="688" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A688" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B688" t="s">
+        <v>18</v>
+      </c>
+      <c r="C688">
+        <v>223.51</v>
+      </c>
+      <c r="D688">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="689" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A689" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B689" t="s">
+        <v>19</v>
+      </c>
+      <c r="C689">
+        <v>1231.53</v>
+      </c>
+      <c r="D689">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="690" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A690" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B690" t="s">
+        <v>20</v>
+      </c>
+      <c r="C690">
+        <v>489.78</v>
+      </c>
+      <c r="D690">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="691" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A691" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B691" t="s">
+        <v>21</v>
+      </c>
+      <c r="C691">
+        <v>496.97</v>
+      </c>
+      <c r="D691">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="692" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A692" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B692" t="s">
+        <v>22</v>
+      </c>
+      <c r="C692">
+        <v>453.62</v>
+      </c>
+      <c r="D692">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="693" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A693" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B693" t="s">
+        <v>23</v>
+      </c>
+      <c r="C693">
+        <v>232.7</v>
+      </c>
+      <c r="D693">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="694" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A694" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B694" t="s">
+        <v>24</v>
+      </c>
+      <c r="C694">
+        <v>552.38</v>
+      </c>
+      <c r="D694">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="695" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A695" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B695" t="s">
+        <v>25</v>
+      </c>
+      <c r="C695">
+        <v>608.83000000000004</v>
+      </c>
+      <c r="D695">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="696" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A696" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B696" t="s">
+        <v>26</v>
+      </c>
+      <c r="C696">
+        <v>432.18</v>
+      </c>
+      <c r="D696">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="697" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A697" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B697" t="s">
+        <v>27</v>
+      </c>
+      <c r="C697">
+        <v>866.57</v>
+      </c>
+      <c r="D697">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="698" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A698" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B698" t="s">
+        <v>28</v>
+      </c>
+      <c r="C698">
+        <v>946.35</v>
+      </c>
+      <c r="D698">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A699" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B699" t="s">
+        <v>29</v>
+      </c>
+      <c r="C699">
+        <v>658.33</v>
+      </c>
+      <c r="D699">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="700" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A700" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B700" t="s">
+        <v>30</v>
+      </c>
+      <c r="C700">
+        <v>238.23</v>
+      </c>
+      <c r="D700">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="701" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A701" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B701" t="s">
+        <v>31</v>
+      </c>
+      <c r="C701">
+        <v>556.01</v>
+      </c>
+      <c r="D701">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="702" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A702" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B702" t="s">
+        <v>32</v>
+      </c>
+      <c r="C702">
+        <v>108.88</v>
+      </c>
+      <c r="D702">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="703" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A703" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B703" t="s">
+        <v>33</v>
+      </c>
+      <c r="C703">
+        <v>185.4</v>
+      </c>
+      <c r="D703">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="704" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A704" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B704" t="s">
+        <v>34</v>
+      </c>
+      <c r="C704">
+        <v>663.54</v>
+      </c>
+      <c r="D704">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="705" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A705" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B705" t="s">
+        <v>35</v>
+      </c>
+      <c r="C705">
+        <v>685.2</v>
+      </c>
+      <c r="D705">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="706" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A706" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B706" t="s">
+        <v>4</v>
+      </c>
+      <c r="C706">
+        <v>2609.41</v>
+      </c>
+      <c r="D706">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="707" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A707" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B707" t="s">
+        <v>5</v>
+      </c>
+      <c r="C707">
+        <v>754.54</v>
+      </c>
+      <c r="D707">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="708" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A708" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B708" t="s">
+        <v>6</v>
+      </c>
+      <c r="C708">
+        <v>395.03</v>
+      </c>
+      <c r="D708">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="709" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A709" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B709" t="s">
+        <v>7</v>
+      </c>
+      <c r="C709">
+        <v>725.25</v>
+      </c>
+      <c r="D709">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="710" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A710" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B710" t="s">
+        <v>8</v>
+      </c>
+      <c r="C710">
+        <v>249.75</v>
+      </c>
+      <c r="D710">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="711" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A711" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B711" t="s">
+        <v>9</v>
+      </c>
+      <c r="C711">
+        <v>781.83</v>
+      </c>
+      <c r="D711">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="712" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A712" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B712" t="s">
+        <v>10</v>
+      </c>
+      <c r="C712">
+        <v>332.8</v>
+      </c>
+      <c r="D712">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="713" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A713" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B713" t="s">
+        <v>11</v>
+      </c>
+      <c r="C713">
+        <v>348.63</v>
+      </c>
+      <c r="D713">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A714" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B714" t="s">
+        <v>12</v>
+      </c>
+      <c r="C714">
+        <v>632.91</v>
+      </c>
+      <c r="D714">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A715" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B715" t="s">
+        <v>13</v>
+      </c>
+      <c r="C715">
+        <v>333.77</v>
+      </c>
+      <c r="D715">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="716" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A716" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B716" t="s">
+        <v>14</v>
+      </c>
+      <c r="C716">
+        <v>960.09</v>
+      </c>
+      <c r="D716">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="717" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A717" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B717" t="s">
+        <v>15</v>
+      </c>
+      <c r="C717">
+        <v>750.56</v>
+      </c>
+      <c r="D717">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="718" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A718" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B718" t="s">
+        <v>16</v>
+      </c>
+      <c r="C718">
+        <v>839.55</v>
+      </c>
+      <c r="D718">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="719" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A719" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B719" t="s">
+        <v>17</v>
+      </c>
+      <c r="C719">
+        <v>759.05</v>
+      </c>
+      <c r="D719">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="720" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A720" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B720" t="s">
+        <v>18</v>
+      </c>
+      <c r="C720">
+        <v>225.22</v>
+      </c>
+      <c r="D720">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="721" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A721" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B721" t="s">
+        <v>19</v>
+      </c>
+      <c r="C721">
+        <v>1234.3900000000001</v>
+      </c>
+      <c r="D721">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="722" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A722" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B722" t="s">
+        <v>20</v>
+      </c>
+      <c r="C722">
+        <v>507</v>
+      </c>
+      <c r="D722">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="723" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A723" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B723" t="s">
+        <v>21</v>
+      </c>
+      <c r="C723">
+        <v>523.08000000000004</v>
+      </c>
+      <c r="D723">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="724" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A724" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B724" t="s">
+        <v>22</v>
+      </c>
+      <c r="C724">
+        <v>472.07</v>
+      </c>
+      <c r="D724">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="725" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A725" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B725" t="s">
+        <v>23</v>
+      </c>
+      <c r="C725">
+        <v>236.27</v>
+      </c>
+      <c r="D725">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="726" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A726" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B726" t="s">
+        <v>24</v>
+      </c>
+      <c r="C726">
+        <v>564.14</v>
+      </c>
+      <c r="D726">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="727" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A727" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B727" t="s">
+        <v>25</v>
+      </c>
+      <c r="C727">
+        <v>641.75</v>
+      </c>
+      <c r="D727">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="728" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A728" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B728" t="s">
+        <v>26</v>
+      </c>
+      <c r="C728">
+        <v>456.77</v>
+      </c>
+      <c r="D728">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="729" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A729" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B729" t="s">
+        <v>27</v>
+      </c>
+      <c r="C729">
+        <v>910.66</v>
+      </c>
+      <c r="D729">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="730" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A730" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B730" t="s">
+        <v>28</v>
+      </c>
+      <c r="C730">
+        <v>1003.47</v>
+      </c>
+      <c r="D730">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="731" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A731" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B731" t="s">
+        <v>29</v>
+      </c>
+      <c r="C731">
+        <v>660.76</v>
+      </c>
+      <c r="D731">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="732" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A732" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B732" t="s">
+        <v>30</v>
+      </c>
+      <c r="C732">
+        <v>238.8</v>
+      </c>
+      <c r="D732">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="733" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A733" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B733" t="s">
+        <v>31</v>
+      </c>
+      <c r="C733">
+        <v>600.76</v>
+      </c>
+      <c r="D733">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="734" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A734" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B734" t="s">
+        <v>32</v>
+      </c>
+      <c r="C734">
+        <v>113.07</v>
+      </c>
+      <c r="D734">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="735" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A735" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B735" t="s">
+        <v>33</v>
+      </c>
+      <c r="C735">
+        <v>188.89</v>
+      </c>
+      <c r="D735">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="736" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A736" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B736" t="s">
+        <v>34</v>
+      </c>
+      <c r="C736">
+        <v>667.22</v>
+      </c>
+      <c r="D736">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="737" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A737" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B737" t="s">
+        <v>35</v>
+      </c>
+      <c r="C737">
+        <v>703.13</v>
+      </c>
+      <c r="D737">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="738" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A738" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B738" t="s">
+        <v>4</v>
+      </c>
+      <c r="C738">
+        <v>2684.95</v>
+      </c>
+      <c r="D738">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="739" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A739" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B739" t="s">
+        <v>5</v>
+      </c>
+      <c r="C739">
+        <v>773.43</v>
+      </c>
+      <c r="D739">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="740" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A740" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B740" t="s">
+        <v>6</v>
+      </c>
+      <c r="C740">
+        <v>398</v>
+      </c>
+      <c r="D740">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="741" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A741" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B741" t="s">
+        <v>7</v>
+      </c>
+      <c r="C741">
+        <v>751.15</v>
+      </c>
+      <c r="D741">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="742" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A742" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B742" t="s">
+        <v>8</v>
+      </c>
+      <c r="C742">
+        <v>249.75</v>
+      </c>
+      <c r="D742">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="743" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A743" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B743" t="s">
+        <v>9</v>
+      </c>
+      <c r="C743">
+        <v>830.01</v>
+      </c>
+      <c r="D743">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="744" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A744" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B744" t="s">
+        <v>10</v>
+      </c>
+      <c r="C744">
+        <v>334.37</v>
+      </c>
+      <c r="D744">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="745" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A745" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B745" t="s">
+        <v>11</v>
+      </c>
+      <c r="C745">
+        <v>368.95</v>
+      </c>
+      <c r="D745">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="746" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A746" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B746" t="s">
+        <v>12</v>
+      </c>
+      <c r="C746">
+        <v>683.77</v>
+      </c>
+      <c r="D746">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="747" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A747" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B747" t="s">
+        <v>13</v>
+      </c>
+      <c r="C747">
+        <v>383.4</v>
+      </c>
+      <c r="D747">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="748" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A748" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B748" t="s">
+        <v>14</v>
+      </c>
+      <c r="C748">
+        <v>1015.55</v>
+      </c>
+      <c r="D748">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="749" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A749" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B749" t="s">
+        <v>15</v>
+      </c>
+      <c r="C749">
+        <v>780.27</v>
+      </c>
+      <c r="D749">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="750" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A750" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B750" t="s">
+        <v>16</v>
+      </c>
+      <c r="C750">
+        <v>888.42</v>
+      </c>
+      <c r="D750">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="751" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A751" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B751" t="s">
+        <v>17</v>
+      </c>
+      <c r="C751">
+        <v>771.1</v>
+      </c>
+      <c r="D751">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="752" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A752" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B752" t="s">
+        <v>18</v>
+      </c>
+      <c r="C752">
+        <v>276.39999999999998</v>
+      </c>
+      <c r="D752">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="753" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A753" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B753" t="s">
+        <v>19</v>
+      </c>
+      <c r="C753">
+        <v>1240.1099999999999</v>
+      </c>
+      <c r="D753">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="754" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A754" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B754" t="s">
+        <v>20</v>
+      </c>
+      <c r="C754">
+        <v>534.36</v>
+      </c>
+      <c r="D754">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="755" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A755" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B755" t="s">
+        <v>21</v>
+      </c>
+      <c r="C755">
+        <v>554.59</v>
+      </c>
+      <c r="D755">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="756" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A756" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B756" t="s">
+        <v>22</v>
+      </c>
+      <c r="C756">
+        <v>490.52</v>
+      </c>
+      <c r="D756">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="757" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A757" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B757" t="s">
+        <v>23</v>
+      </c>
+      <c r="C757">
+        <v>254.99</v>
+      </c>
+      <c r="D757">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="758" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A758" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B758" t="s">
+        <v>24</v>
+      </c>
+      <c r="C758">
+        <v>587.20000000000005</v>
+      </c>
+      <c r="D758">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="759" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A759" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B759" t="s">
+        <v>25</v>
+      </c>
+      <c r="C759">
+        <v>699.03</v>
+      </c>
+      <c r="D759">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="760" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A760" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B760" t="s">
+        <v>26</v>
+      </c>
+      <c r="C760">
+        <v>485.96</v>
+      </c>
+      <c r="D760">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="761" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A761" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B761" t="s">
+        <v>27</v>
+      </c>
+      <c r="C761">
+        <v>948.82</v>
+      </c>
+      <c r="D761">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="762" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A762" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B762" t="s">
+        <v>28</v>
+      </c>
+      <c r="C762">
+        <v>1081.26</v>
+      </c>
+      <c r="D762">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="763" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A763" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B763" t="s">
+        <v>29</v>
+      </c>
+      <c r="C763">
+        <v>665.32</v>
+      </c>
+      <c r="D763">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="764" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A764" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B764" t="s">
+        <v>30</v>
+      </c>
+      <c r="C764">
+        <v>279.54000000000002</v>
+      </c>
+      <c r="D764">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="765" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A765" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B765" t="s">
+        <v>31</v>
+      </c>
+      <c r="C765">
+        <v>639.78</v>
+      </c>
+      <c r="D765">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="766" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A766" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B766" t="s">
+        <v>32</v>
+      </c>
+      <c r="C766">
+        <v>121.97</v>
+      </c>
+      <c r="D766">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="767" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A767" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B767" t="s">
+        <v>33</v>
+      </c>
+      <c r="C767">
+        <v>204.05</v>
+      </c>
+      <c r="D767">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="768" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A768" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B768" t="s">
+        <v>34</v>
+      </c>
+      <c r="C768">
+        <v>707.66</v>
+      </c>
+      <c r="D768">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="769" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A769" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B769" t="s">
+        <v>35</v>
+      </c>
+      <c r="C769">
+        <v>723.43</v>
+      </c>
+      <c r="D769">
+        <v>423</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9760,7 +11608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F422A3AD-6985-4C77-AE63-323FE7C4AE0C}">
   <dimension ref="A1:E127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+    <sheetView topLeftCell="A102" workbookViewId="0">
       <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add this week's data
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4235A80-B4F4-4924-BD3A-37C1B7FC0648}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F63B36-F262-4729-8CAC-A466B12976CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="9360" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="9360" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fallecido_Recuperado" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,6 +1004,20 @@
         <v>103412</v>
       </c>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B33">
+        <v>128278</v>
+      </c>
+      <c r="C33">
+        <v>2257</v>
+      </c>
+      <c r="D33">
+        <v>106304</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1011,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D993"/>
+  <dimension ref="A1:D1025"/>
   <sheetViews>
-    <sheetView topLeftCell="A968" workbookViewId="0">
-      <selection activeCell="D994" sqref="D994"/>
+    <sheetView tabSelected="1" topLeftCell="A1000" workbookViewId="0">
+      <selection activeCell="D1026" sqref="D1026"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14829,6 +14843,454 @@
       </c>
       <c r="D993">
         <v>478</v>
+      </c>
+    </row>
+    <row r="994" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A994" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B994" t="s">
+        <v>4</v>
+      </c>
+      <c r="C994">
+        <v>3210.26</v>
+      </c>
+      <c r="D994">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="995" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A995" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B995" t="s">
+        <v>5</v>
+      </c>
+      <c r="C995">
+        <v>916.96</v>
+      </c>
+      <c r="D995">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="996" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A996" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B996" t="s">
+        <v>6</v>
+      </c>
+      <c r="C996">
+        <v>932.63</v>
+      </c>
+      <c r="D996">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="997" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A997" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B997" t="s">
+        <v>7</v>
+      </c>
+      <c r="C997">
+        <v>1070.95</v>
+      </c>
+      <c r="D997">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="998" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A998" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B998" t="s">
+        <v>8</v>
+      </c>
+      <c r="C998">
+        <v>547.64</v>
+      </c>
+      <c r="D998">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="999" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A999" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B999" t="s">
+        <v>9</v>
+      </c>
+      <c r="C999">
+        <v>1082.92</v>
+      </c>
+      <c r="D999">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1000" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1000">
+        <v>367.5</v>
+      </c>
+      <c r="D1000">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1001" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1001">
+        <v>581.77</v>
+      </c>
+      <c r="D1001">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1002" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1002">
+        <v>1112.3900000000001</v>
+      </c>
+      <c r="D1002">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1003" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1003">
+        <v>1136.52</v>
+      </c>
+      <c r="D1003">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1004" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1004">
+        <v>1352.55</v>
+      </c>
+      <c r="D1004">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1005" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1005">
+        <v>1177.93</v>
+      </c>
+      <c r="D1005">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1006" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1006">
+        <v>1165.5999999999999</v>
+      </c>
+      <c r="D1006">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1007" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1007">
+        <v>868.91</v>
+      </c>
+      <c r="D1007">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1008" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1008">
+        <v>516.12</v>
+      </c>
+      <c r="D1008">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1009" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1009">
+        <v>1577.28</v>
+      </c>
+      <c r="D1009">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1010" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1010">
+        <v>663.51</v>
+      </c>
+      <c r="D1010">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1011" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1011">
+        <v>987.63</v>
+      </c>
+      <c r="D1011">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1012" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1012">
+        <v>1014.67</v>
+      </c>
+      <c r="D1012">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1013" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1013">
+        <v>445.79</v>
+      </c>
+      <c r="D1013">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1014" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1014">
+        <v>740.16</v>
+      </c>
+      <c r="D1014">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1015" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1015">
+        <v>1013.82</v>
+      </c>
+      <c r="D1015">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1016" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1016">
+        <v>568.59</v>
+      </c>
+      <c r="D1016">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1017" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1017">
+        <v>1269.26</v>
+      </c>
+      <c r="D1017">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1018" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1018">
+        <v>1354.8</v>
+      </c>
+      <c r="D1018">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1019" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1019">
+        <v>1105.3699999999999</v>
+      </c>
+      <c r="D1019">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1020" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1020">
+        <v>534.74</v>
+      </c>
+      <c r="D1020">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1021" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1021">
+        <v>945.04</v>
+      </c>
+      <c r="D1021">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1022" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1022">
+        <v>301</v>
+      </c>
+      <c r="D1022">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1023" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1023">
+        <v>544.53</v>
+      </c>
+      <c r="D1023">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1024" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1024">
+        <v>985.2</v>
+      </c>
+      <c r="D1024">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1025" s="2">
+        <v>44138</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1025">
+        <v>889.3</v>
+      </c>
+      <c r="D1025">
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two more weeks of data
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00BDA64-B805-45F8-8860-8E6CEE783827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E776E7-371C-4399-A2CF-E565089197AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="240" windowWidth="9360" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,6 +1032,34 @@
         <v>109057</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B35">
+        <v>135157</v>
+      </c>
+      <c r="C35">
+        <v>2293</v>
+      </c>
+      <c r="D35">
+        <v>110871</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B36">
+        <v>138410</v>
+      </c>
+      <c r="C36">
+        <v>2310</v>
+      </c>
+      <c r="D36">
+        <v>112552</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1039,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D1057"/>
+  <dimension ref="A1:D1121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1032" workbookViewId="0">
-      <selection activeCell="D1058" sqref="D1058"/>
+    <sheetView tabSelected="1" topLeftCell="A1096" workbookViewId="0">
+      <selection activeCell="D1122" sqref="D1122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15753,6 +15781,902 @@
       </c>
       <c r="D1057">
         <v>487</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1058" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1058">
+        <v>3383.86</v>
+      </c>
+      <c r="D1058">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1059" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1059">
+        <v>927.31</v>
+      </c>
+      <c r="D1059">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1060" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1060">
+        <v>977.31</v>
+      </c>
+      <c r="D1060">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1061" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1061">
+        <v>1096.33</v>
+      </c>
+      <c r="D1061">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1062" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1062">
+        <v>606.32000000000005</v>
+      </c>
+      <c r="D1062">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1063" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1063">
+        <v>1192.6500000000001</v>
+      </c>
+      <c r="D1063">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1064" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1064">
+        <v>372.23</v>
+      </c>
+      <c r="D1064">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1065" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1065">
+        <v>584.98</v>
+      </c>
+      <c r="D1065">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1066" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1066">
+        <v>1162.42</v>
+      </c>
+      <c r="D1066">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1067" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1067">
+        <v>1177.5999999999999</v>
+      </c>
+      <c r="D1067">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1068" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1068">
+        <v>1401.79</v>
+      </c>
+      <c r="D1068">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1069" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1069">
+        <v>1230.75</v>
+      </c>
+      <c r="D1069">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1070" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1070">
+        <v>1258.97</v>
+      </c>
+      <c r="D1070">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1071" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1071">
+        <v>901.51</v>
+      </c>
+      <c r="D1071">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1072" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1072">
+        <v>560.48</v>
+      </c>
+      <c r="D1072">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1073" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1073">
+        <v>1611.57</v>
+      </c>
+      <c r="D1073">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1074" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1074">
+        <v>686.81</v>
+      </c>
+      <c r="D1074">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1075" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1075">
+        <v>1084.57</v>
+      </c>
+      <c r="D1075">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1076" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1076">
+        <v>1071.0999999999999</v>
+      </c>
+      <c r="D1076">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1077" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1077">
+        <v>487.7</v>
+      </c>
+      <c r="D1077">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1078" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1078">
+        <v>767.14</v>
+      </c>
+      <c r="D1078">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1079" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1079">
+        <v>1041.33</v>
+      </c>
+      <c r="D1079">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1080" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1080">
+        <v>584.33000000000004</v>
+      </c>
+      <c r="D1080">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1081" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1081">
+        <v>1342.3</v>
+      </c>
+      <c r="D1081">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1082" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1082">
+        <v>1408.67</v>
+      </c>
+      <c r="D1082">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1083" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1083">
+        <v>1169.98</v>
+      </c>
+      <c r="D1083">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1084" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1084">
+        <v>550.02</v>
+      </c>
+      <c r="D1084">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1085" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1085">
+        <v>1086.2</v>
+      </c>
+      <c r="D1085">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1086" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1086">
+        <v>312.51</v>
+      </c>
+      <c r="D1086">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1087" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1087">
+        <v>569.02</v>
+      </c>
+      <c r="D1087">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1088" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1088">
+        <v>1060.56</v>
+      </c>
+      <c r="D1088">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1089" s="2">
+        <v>44149</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1089">
+        <v>941.88</v>
+      </c>
+      <c r="D1089">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1090" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1090">
+        <v>3485.67</v>
+      </c>
+      <c r="D1090">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1091" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1091">
+        <v>929.11</v>
+      </c>
+      <c r="D1091">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1092" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1092">
+        <v>979.16</v>
+      </c>
+      <c r="D1092">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1093" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1093">
+        <v>1097.3800000000001</v>
+      </c>
+      <c r="D1093">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1094" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1094">
+        <v>655.96</v>
+      </c>
+      <c r="D1094">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1095" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1095">
+        <v>1257.22</v>
+      </c>
+      <c r="D1095">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1096" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1096">
+        <v>375.38</v>
+      </c>
+      <c r="D1096">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1097" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1097">
+        <v>586.04999999999995</v>
+      </c>
+      <c r="D1097">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1098" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1098">
+        <v>1183.26</v>
+      </c>
+      <c r="D1098">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1099" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1099">
+        <v>1223.81</v>
+      </c>
+      <c r="D1099">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1100" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1100">
+        <v>1429.8</v>
+      </c>
+      <c r="D1100">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1101" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1101">
+        <v>1245.06</v>
+      </c>
+      <c r="D1101">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1102" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1102">
+        <v>1307.1099999999999</v>
+      </c>
+      <c r="D1102">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1103" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1103">
+        <v>930.57</v>
+      </c>
+      <c r="D1103">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1104" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1104">
+        <v>561.33000000000004</v>
+      </c>
+      <c r="D1104">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1105" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1105">
+        <v>1611.57</v>
+      </c>
+      <c r="D1105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1106" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1106">
+        <v>689.85</v>
+      </c>
+      <c r="D1106">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1107" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1107">
+        <v>1139.18</v>
+      </c>
+      <c r="D1107">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1108" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1108">
+        <v>1078.7</v>
+      </c>
+      <c r="D1108">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1109" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1109">
+        <v>499.29</v>
+      </c>
+      <c r="D1109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1110" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1110">
+        <v>778.28</v>
+      </c>
+      <c r="D1110">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1111" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1111">
+        <v>1049.9000000000001</v>
+      </c>
+      <c r="D1111">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1112" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1112">
+        <v>604.99</v>
+      </c>
+      <c r="D1112">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1113" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1113">
+        <v>1396.91</v>
+      </c>
+      <c r="D1113">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1114" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1114">
+        <v>1430.68</v>
+      </c>
+      <c r="D1114">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1115" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1115">
+        <v>1185.69</v>
+      </c>
+      <c r="D1115">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1116" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1116">
+        <v>552.85</v>
+      </c>
+      <c r="D1116">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1117" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1117">
+        <v>1152.18</v>
+      </c>
+      <c r="D1117">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1118" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1118">
+        <v>316.18</v>
+      </c>
+      <c r="D1118">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1119" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1119">
+        <v>571.35</v>
+      </c>
+      <c r="D1119">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1120" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1120">
+        <v>1062.4000000000001</v>
+      </c>
+      <c r="D1120">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1121" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1121">
+        <v>964.62</v>
+      </c>
+      <c r="D1121">
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two more weeks of data, mid-December
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E22EC3-FB70-469A-82A0-B6F3748CCB2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4AD816-54F3-471D-97BC-4D28AC582B59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="9360" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="11700" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fallecido_Recuperado" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,6 +1102,39 @@
         <v>119616</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B40">
+        <v>159064</v>
+      </c>
+      <c r="C40">
+        <v>2382</v>
+      </c>
+      <c r="D40">
+        <v>123284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B41">
+        <v>165940</v>
+      </c>
+      <c r="C41">
+        <v>2404</v>
+      </c>
+      <c r="D41">
+        <v>127866</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>44197</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1109,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D1217"/>
+  <dimension ref="A1:D1282"/>
   <sheetViews>
-    <sheetView topLeftCell="A1192" workbookViewId="0">
-      <selection activeCell="D1218" sqref="D1218"/>
+    <sheetView topLeftCell="A1256" workbookViewId="0">
+      <selection activeCell="D1282" sqref="D1282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18063,6 +18096,907 @@
       </c>
       <c r="D1217">
         <v>481</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1218" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1218">
+        <v>4077.22</v>
+      </c>
+      <c r="D1218">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1219" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1219">
+        <v>970.95</v>
+      </c>
+      <c r="D1219">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1220" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1220">
+        <v>1018.76</v>
+      </c>
+      <c r="D1220">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1221" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1221">
+        <v>1162.4000000000001</v>
+      </c>
+      <c r="D1221">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1222" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1222">
+        <v>761.28</v>
+      </c>
+      <c r="D1222">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1223" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1223">
+        <v>1604.48</v>
+      </c>
+      <c r="D1223">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1224" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1224">
+        <v>410.08</v>
+      </c>
+      <c r="D1224">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1225" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1225">
+        <v>632.03</v>
+      </c>
+      <c r="D1225">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1226" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1226">
+        <v>1294.17</v>
+      </c>
+      <c r="D1226">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1227" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1227">
+        <v>1314.53</v>
+      </c>
+      <c r="D1227">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1228" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1228">
+        <v>1615.14</v>
+      </c>
+      <c r="D1228">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1229" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1229">
+        <v>1896.57</v>
+      </c>
+      <c r="D1229">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1230" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1230" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1230">
+        <v>1549.76</v>
+      </c>
+      <c r="D1230">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1231" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1231">
+        <v>1081.53</v>
+      </c>
+      <c r="D1231">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1232" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1232">
+        <v>584.37</v>
+      </c>
+      <c r="D1232">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1233" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1233">
+        <v>1620.14</v>
+      </c>
+      <c r="D1233">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1234" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1234">
+        <v>746.07</v>
+      </c>
+      <c r="D1234">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1235" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1235" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1235">
+        <v>1375.96</v>
+      </c>
+      <c r="D1235">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1236" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1236" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1236">
+        <v>1276.21</v>
+      </c>
+      <c r="D1236">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1237" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1237" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1237">
+        <v>530.49</v>
+      </c>
+      <c r="D1237">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1238" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1238" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1238">
+        <v>849.66</v>
+      </c>
+      <c r="D1238">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1239" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1239" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1239">
+        <v>1114.3900000000001</v>
+      </c>
+      <c r="D1239">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1240" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1240" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1240">
+        <v>660.4</v>
+      </c>
+      <c r="D1240">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1241" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1241">
+        <v>1527.19</v>
+      </c>
+      <c r="D1241">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1242" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1242">
+        <v>1571.8</v>
+      </c>
+      <c r="D1242">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1243" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1243">
+        <v>1327.14</v>
+      </c>
+      <c r="D1243">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1244" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1244">
+        <v>649.62</v>
+      </c>
+      <c r="D1244">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1245" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1245">
+        <v>1473.51</v>
+      </c>
+      <c r="D1245">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1246" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1246">
+        <v>352.3</v>
+      </c>
+      <c r="D1246">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1247" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1247">
+        <v>609.83000000000004</v>
+      </c>
+      <c r="D1247">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1248" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1248">
+        <v>1185.55</v>
+      </c>
+      <c r="D1248">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1249" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1249">
+        <v>1116</v>
+      </c>
+      <c r="D1249">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1250" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1250">
+        <v>4329.72</v>
+      </c>
+      <c r="D1250">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1251" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1251">
+        <v>986.7</v>
+      </c>
+      <c r="D1251">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1252" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1252">
+        <v>1037.57</v>
+      </c>
+      <c r="D1252">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1253" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1253">
+        <v>1176.68</v>
+      </c>
+      <c r="D1253">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1254" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1254">
+        <v>807.92</v>
+      </c>
+      <c r="D1254">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1255" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1255">
+        <v>1666.04</v>
+      </c>
+      <c r="D1255">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1256" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1256">
+        <v>414.81</v>
+      </c>
+      <c r="D1256">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1257" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1257">
+        <v>634.16999999999996</v>
+      </c>
+      <c r="D1257">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1258" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1258">
+        <v>1330.44</v>
+      </c>
+      <c r="D1258">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1259" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1259">
+        <v>1355.61</v>
+      </c>
+      <c r="D1259">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1260" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1260">
+        <v>1696.92</v>
+      </c>
+      <c r="D1260">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1261" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1261">
+        <v>1922.25</v>
+      </c>
+      <c r="D1261">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1262" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1262">
+        <v>1619.3</v>
+      </c>
+      <c r="D1262">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1263" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1263">
+        <v>1165.1600000000001</v>
+      </c>
+      <c r="D1263">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1264" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1264">
+        <v>603.99</v>
+      </c>
+      <c r="D1264">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1265" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1265">
+        <v>1637.28</v>
+      </c>
+      <c r="D1265">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1266" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1266">
+        <v>768.36</v>
+      </c>
+      <c r="D1266">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1267" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1267">
+        <v>1451.59</v>
+      </c>
+      <c r="D1267">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1268" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1268">
+        <v>1319.62</v>
+      </c>
+      <c r="D1268">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1269" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1269">
+        <v>548.32000000000005</v>
+      </c>
+      <c r="D1269">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1270" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1270">
+        <v>863.78</v>
+      </c>
+      <c r="D1270">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1271" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1271">
+        <v>1145.96</v>
+      </c>
+      <c r="D1271">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1272" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1272">
+        <v>682.37</v>
+      </c>
+      <c r="D1272">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1273" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1273">
+        <v>1560.75</v>
+      </c>
+      <c r="D1273">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1274" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1274">
+        <v>1656.96</v>
+      </c>
+      <c r="D1274">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1275" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1275" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1275">
+        <v>1348.09</v>
+      </c>
+      <c r="D1275">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1276" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1276" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1276">
+        <v>677.34</v>
+      </c>
+      <c r="D1276">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1277" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1277" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1277">
+        <v>1535.48</v>
+      </c>
+      <c r="D1277">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1278" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1278" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1278">
+        <v>362.24</v>
+      </c>
+      <c r="D1278">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1279" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1279" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1279">
+        <v>617.99</v>
+      </c>
+      <c r="D1279">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1280" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1280" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1280">
+        <v>1205.77</v>
+      </c>
+      <c r="D1280">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1281" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B1281" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1281">
+        <v>1156.19</v>
+      </c>
+      <c r="D1281">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1282" s="2">
+        <v>44197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Another week of data, plus image of 2020 total
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4AD816-54F3-471D-97BC-4D28AC582B59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA2B084-9D47-4643-B82B-60726EE86E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="105" windowWidth="11700" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,6 +1134,20 @@
       <c r="A42" s="2">
         <v>44197</v>
       </c>
+      <c r="B42">
+        <v>172965</v>
+      </c>
+      <c r="C42">
+        <v>2416</v>
+      </c>
+      <c r="D42">
+        <v>132282</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>44204</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1142,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D1282"/>
+  <dimension ref="A1:D1314"/>
   <sheetViews>
-    <sheetView topLeftCell="A1256" workbookViewId="0">
-      <selection activeCell="D1282" sqref="D1282"/>
+    <sheetView topLeftCell="A1288" workbookViewId="0">
+      <selection activeCell="B1314" sqref="B1314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18997,6 +19011,454 @@
     <row r="1282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1282" s="2">
         <v>44197</v>
+      </c>
+      <c r="B1282" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1282">
+        <v>4592.57</v>
+      </c>
+      <c r="D1282">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1283" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1283" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1283">
+        <v>996.6</v>
+      </c>
+      <c r="D1283">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1284" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1284" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1284">
+        <v>1053.4100000000001</v>
+      </c>
+      <c r="D1284">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1285" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1285" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1285">
+        <v>1188.31</v>
+      </c>
+      <c r="D1285">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1286" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1286" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1286">
+        <v>842.52</v>
+      </c>
+      <c r="D1286">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1287" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1287" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1287">
+        <v>1720.9</v>
+      </c>
+      <c r="D1287">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1288" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1288" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1288">
+        <v>425.85</v>
+      </c>
+      <c r="D1288">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1289" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1289" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1289">
+        <v>638.45000000000005</v>
+      </c>
+      <c r="D1289">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1290" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1290" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1290">
+        <v>1362.55</v>
+      </c>
+      <c r="D1290">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1291" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1291" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1291">
+        <v>1371.01</v>
+      </c>
+      <c r="D1291">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1292" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1292" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1292">
+        <v>1778.12</v>
+      </c>
+      <c r="D1292">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1293" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1293" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1293">
+        <v>1950.5</v>
+      </c>
+      <c r="D1293">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1294" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1294" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1294">
+        <v>1699.29</v>
+      </c>
+      <c r="D1294">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1295" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1295" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1295">
+        <v>1265.8</v>
+      </c>
+      <c r="D1295">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1296" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1296" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1296">
+        <v>607.4</v>
+      </c>
+      <c r="D1296">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1297" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1297" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1297">
+        <v>1637.28</v>
+      </c>
+      <c r="D1297">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1298" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1298" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1298">
+        <v>793.18</v>
+      </c>
+      <c r="D1298">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1299" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1299" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1299">
+        <v>1532.02</v>
+      </c>
+      <c r="D1299">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1300" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1300" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1300">
+        <v>1379.3</v>
+      </c>
+      <c r="D1300">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1301" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1301" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1301">
+        <v>556.35</v>
+      </c>
+      <c r="D1301">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1302" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1302" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1302">
+        <v>878.84</v>
+      </c>
+      <c r="D1302">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1303" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1303" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1303">
+        <v>1177.53</v>
+      </c>
+      <c r="D1303">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1304" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1304" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1304">
+        <v>702.05</v>
+      </c>
+      <c r="D1304">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1305" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1305" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1305">
+        <v>1606.81</v>
+      </c>
+      <c r="D1305">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1306" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1306" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1306">
+        <v>1723.74</v>
+      </c>
+      <c r="D1306">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1307" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1307" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1307">
+        <v>1381.27</v>
+      </c>
+      <c r="D1307">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1308" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1308" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1308">
+        <v>718.09</v>
+      </c>
+      <c r="D1308">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1309" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1309" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1309">
+        <v>1583.68</v>
+      </c>
+      <c r="D1309">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1310" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1310" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1310">
+        <v>386.32</v>
+      </c>
+      <c r="D1310">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1311" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1311" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1311">
+        <v>642.48</v>
+      </c>
+      <c r="D1311">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1312" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1312">
+        <v>1231.5</v>
+      </c>
+      <c r="D1312">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1313" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B1313" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1313">
+        <v>1199.3399999999999</v>
+      </c>
+      <c r="D1313">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1314" s="2">
+        <v>44204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest date 5 February
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7E8C10-C746-404E-8865-3BD0E1D97CF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09CEFD-28E5-4F0E-9D47-6DCF51845B56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="11700" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
+    <workbookView xWindow="735" yWindow="450" windowWidth="10170" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fallecido_Recuperado" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,6 +1190,34 @@
       <c r="A46" s="2">
         <v>44225</v>
       </c>
+      <c r="B46">
+        <v>212553</v>
+      </c>
+      <c r="C46">
+        <v>2646</v>
+      </c>
+      <c r="D46">
+        <v>155867</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B47">
+        <v>222148</v>
+      </c>
+      <c r="C47">
+        <v>2801</v>
+      </c>
+      <c r="D47">
+        <v>165659</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>44239</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1198,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D1410"/>
+  <dimension ref="A1:D1473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1384" workbookViewId="0">
-      <selection activeCell="B1410" sqref="B1410"/>
+    <sheetView tabSelected="1" topLeftCell="A1448" workbookViewId="0">
+      <selection activeCell="A1474" sqref="A1474"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20845,6 +20873,897 @@
     <row r="1410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1410" s="2">
         <v>44225</v>
+      </c>
+      <c r="B1410" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1410">
+        <v>5727.07</v>
+      </c>
+      <c r="D1410">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1411" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1411" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1411">
+        <v>1113.1300000000001</v>
+      </c>
+      <c r="D1411">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1412" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1412" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1412">
+        <v>1228.6500000000001</v>
+      </c>
+      <c r="D1412">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1413" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1413" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1413">
+        <v>1282.4000000000001</v>
+      </c>
+      <c r="D1413">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1414" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1414" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1414">
+        <v>1223.1600000000001</v>
+      </c>
+      <c r="D1414">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1415" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1415" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1415">
+        <v>1958.76</v>
+      </c>
+      <c r="D1415">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1416" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1416" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1416">
+        <v>567.80999999999995</v>
+      </c>
+      <c r="D1416">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1417" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1417" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1417">
+        <v>811.7</v>
+      </c>
+      <c r="D1417">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1418" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1418" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1418">
+        <v>1870.37</v>
+      </c>
+      <c r="D1418">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1419" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1419" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1419">
+        <v>1489.11</v>
+      </c>
+      <c r="D1419">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1420" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1420" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1420">
+        <v>2255.7600000000002</v>
+      </c>
+      <c r="D1420">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1421" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1421" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1421">
+        <v>2263.0500000000002</v>
+      </c>
+      <c r="D1421">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1422" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1422" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1422">
+        <v>2156.87</v>
+      </c>
+      <c r="D1422">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1423" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1423" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1423">
+        <v>1924.92</v>
+      </c>
+      <c r="D1423">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1424" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1424" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1424">
+        <v>789.11</v>
+      </c>
+      <c r="D1424">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1425" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1425" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1425">
+        <v>1723</v>
+      </c>
+      <c r="D1425">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1426" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1426" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1426">
+        <v>892.45</v>
+      </c>
+      <c r="D1426">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1427" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1427" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1427">
+        <v>2084.1999999999998</v>
+      </c>
+      <c r="D1427">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1428" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1428" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1428">
+        <v>2039.11</v>
+      </c>
+      <c r="D1428">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1429" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1429" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1429">
+        <v>678.5</v>
+      </c>
+      <c r="D1429">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1430" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1430" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1430">
+        <v>1005.45</v>
+      </c>
+      <c r="D1430">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1431" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1431" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1431">
+        <v>1407.98</v>
+      </c>
+      <c r="D1431">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1432" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1432" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1432">
+        <v>879.77</v>
+      </c>
+      <c r="D1432">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1433" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1433" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1433">
+        <v>1855.56</v>
+      </c>
+      <c r="D1433">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1434" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1434" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1434">
+        <v>2255.52</v>
+      </c>
+      <c r="D1434">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1435" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1435" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1435">
+        <v>1650.19</v>
+      </c>
+      <c r="D1435">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1436" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1436" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1436">
+        <v>1126.08</v>
+      </c>
+      <c r="D1436">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1437" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1437" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1437">
+        <v>1829.26</v>
+      </c>
+      <c r="D1437">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1438" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1438" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1438">
+        <v>533.94000000000005</v>
+      </c>
+      <c r="D1438">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1439" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1439" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1439">
+        <v>678.62</v>
+      </c>
+      <c r="D1439">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1440" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1440" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1440">
+        <v>1373.04</v>
+      </c>
+      <c r="D1440">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1441" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B1441" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1441">
+        <v>1426.05</v>
+      </c>
+      <c r="D1441">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1442" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1442" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1442">
+        <v>6006.22</v>
+      </c>
+      <c r="D1442">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1443" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1443" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1443">
+        <v>1146.8800000000001</v>
+      </c>
+      <c r="D1443">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1444" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1444" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1444">
+        <v>1262.31</v>
+      </c>
+      <c r="D1444">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1445" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1445" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1445">
+        <v>1318.34</v>
+      </c>
+      <c r="D1445">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1446" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1446" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1446">
+        <v>1314.94</v>
+      </c>
+      <c r="D1446">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1447" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1447" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1447">
+        <v>2009.61</v>
+      </c>
+      <c r="D1447">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1448" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1448" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1448">
+        <v>607.24</v>
+      </c>
+      <c r="D1448">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1449" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1449" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1449">
+        <v>853.4</v>
+      </c>
+      <c r="D1449">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1450" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1450" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1450">
+        <v>1962.1</v>
+      </c>
+      <c r="D1450">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1451" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1451" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1451">
+        <v>1533.62</v>
+      </c>
+      <c r="D1451">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1452" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1452" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1452">
+        <v>2355.9299999999998</v>
+      </c>
+      <c r="D1452">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1453" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1453" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1453">
+        <v>2365.0300000000002</v>
+      </c>
+      <c r="D1453">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1454" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1454" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1454">
+        <v>2245.13</v>
+      </c>
+      <c r="D1454">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1455" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1455" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1455">
+        <v>2012.8</v>
+      </c>
+      <c r="D1455">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1456" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1456" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1456">
+        <v>830.91</v>
+      </c>
+      <c r="D1456">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1457" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1457" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1457">
+        <v>1725.86</v>
+      </c>
+      <c r="D1457">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1458" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1458" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1458">
+        <v>913.72</v>
+      </c>
+      <c r="D1458">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1459" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1459" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1459">
+        <v>2154.13</v>
+      </c>
+      <c r="D1459">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1460" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1460" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1460">
+        <v>2199.7199999999998</v>
+      </c>
+      <c r="D1460">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1461" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1461" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1461">
+        <v>718.62</v>
+      </c>
+      <c r="D1461">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1462" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1462" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1462">
+        <v>1035.4100000000001</v>
+      </c>
+      <c r="D1462">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1463" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1463" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1463">
+        <v>1463.45</v>
+      </c>
+      <c r="D1463">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1464" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1464" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1464">
+        <v>930.6</v>
+      </c>
+      <c r="D1464">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1465" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1465" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1465">
+        <v>1906.85</v>
+      </c>
+      <c r="D1465">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1466" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1466" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1466">
+        <v>2406.88</v>
+      </c>
+      <c r="D1466">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1467" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1467" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1467">
+        <v>1772.43</v>
+      </c>
+      <c r="D1467">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1468" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1468" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1468">
+        <v>1197.94</v>
+      </c>
+      <c r="D1468">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1469" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1469" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1469">
+        <v>1879.76</v>
+      </c>
+      <c r="D1469">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1470" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1470" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1470">
+        <v>554.88</v>
+      </c>
+      <c r="D1470">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1471" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1471" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1471">
+        <v>705.44</v>
+      </c>
+      <c r="D1471">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1472" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1472" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1472">
+        <v>1404.28</v>
+      </c>
+      <c r="D1472">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1473" s="2">
+        <v>44232</v>
+      </c>
+      <c r="B1473" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1473">
+        <v>1489.88</v>
+      </c>
+      <c r="D1473">
+        <v>549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beginning final month: March
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4755802A-9B77-4FE5-8FC7-7D7E235CA5CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580DC5F9-818F-41D7-BA1A-B3F348B98CED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="450" windowWidth="10170" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,6 +1260,20 @@
       <c r="A51" s="2">
         <v>44260</v>
       </c>
+      <c r="B51">
+        <v>242660</v>
+      </c>
+      <c r="C51">
+        <v>3162</v>
+      </c>
+      <c r="D51">
+        <v>196484</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>44267</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1268,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D1569"/>
+  <dimension ref="A1:D1602"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1544" workbookViewId="0">
-      <selection activeCell="A1570" sqref="A1570"/>
+    <sheetView tabSelected="1" topLeftCell="A1576" workbookViewId="0">
+      <selection activeCell="B1602" sqref="B1602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23150,6 +23164,459 @@
       </c>
       <c r="D1569">
         <v>617</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1570" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1570" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1570">
+        <v>6626.91</v>
+      </c>
+      <c r="D1570">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1571" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1571" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1571">
+        <v>1318.3</v>
+      </c>
+      <c r="D1571">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1572" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1572" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1572">
+        <v>1330.63</v>
+      </c>
+      <c r="D1572">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1573" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1573" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1573">
+        <v>1377.02</v>
+      </c>
+      <c r="D1573">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1574" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1574" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1574">
+        <v>1501.5</v>
+      </c>
+      <c r="D1574">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1575" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1575" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1575">
+        <v>2113.66</v>
+      </c>
+      <c r="D1575">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1576" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1576" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1576">
+        <v>635.63</v>
+      </c>
+      <c r="D1576">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1577" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1577" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1577">
+        <v>931.47</v>
+      </c>
+      <c r="D1577">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1578" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1578" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1578">
+        <v>2118.87</v>
+      </c>
+      <c r="D1578">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1579" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1579" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1579">
+        <v>1648.3</v>
+      </c>
+      <c r="D1579">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1580" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1580" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1580">
+        <v>2544.9499999999998</v>
+      </c>
+      <c r="D1580">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1581" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1581" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1581">
+        <v>2691.89</v>
+      </c>
+      <c r="D1581">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1582" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1582" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1582">
+        <v>2402.9299999999998</v>
+      </c>
+      <c r="D1582">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1583" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1583" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1583">
+        <v>2153.84</v>
+      </c>
+      <c r="D1583">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1584" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1584" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1584">
+        <v>943.52</v>
+      </c>
+      <c r="D1584">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1585" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1585" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1585">
+        <v>1791.58</v>
+      </c>
+      <c r="D1585">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1586" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1586" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1586">
+        <v>1019.07</v>
+      </c>
+      <c r="D1586">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1587" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1587" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1587">
+        <v>2255.2600000000002</v>
+      </c>
+      <c r="D1587">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1588" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1588" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1588">
+        <v>2486.2199999999998</v>
+      </c>
+      <c r="D1588">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1589" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1589" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1589">
+        <v>778.35</v>
+      </c>
+      <c r="D1589">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1590" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1590" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1590">
+        <v>1126.56</v>
+      </c>
+      <c r="D1590">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1591" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1591" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1591">
+        <v>1621.75</v>
+      </c>
+      <c r="D1591">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1592" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1592" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1592">
+        <v>1055.8599999999999</v>
+      </c>
+      <c r="D1592">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1593" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1593" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1593">
+        <v>2025.95</v>
+      </c>
+      <c r="D1593">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1594" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1594" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1594">
+        <v>2600.35</v>
+      </c>
+      <c r="D1594">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1595" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1595" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1595">
+        <v>1955.79</v>
+      </c>
+      <c r="D1595">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1596" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1596" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1596">
+        <v>1371.66</v>
+      </c>
+      <c r="D1596">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1597" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1597" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1597">
+        <v>1963.53</v>
+      </c>
+      <c r="D1597">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1598" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1598" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1598">
+        <v>614.54999999999995</v>
+      </c>
+      <c r="D1598">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1599" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1599" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1599">
+        <v>907.16</v>
+      </c>
+      <c r="D1599">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1600" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1600" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1600">
+        <v>1461.26</v>
+      </c>
+      <c r="D1600">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1601" s="2">
+        <v>44260</v>
+      </c>
+      <c r="B1601" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1601">
+        <v>1651.27</v>
+      </c>
+      <c r="D1601">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1602" s="2">
+        <v>44267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final data - one years worth
</commit_message>
<xml_diff>
--- a/Covid_Dominican/Dominican_Covid.xlsx
+++ b/Covid_Dominican/Dominican_Covid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\UC-Berkeley\Covid_Dominican\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965EB7A3-3312-4555-9BDB-628013A89DB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A712F7AE-9F8A-4CBD-BF33-C6FAACBF6096}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="450" windowWidth="10170" windowHeight="12435" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
+    <workbookView xWindow="735" yWindow="450" windowWidth="10170" windowHeight="12435" firstSheet="1" activeTab="1" xr2:uid="{FCFD829C-D18B-42C2-8A3F-F17054977C8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fallecido_Recuperado" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="52">
   <si>
     <t>Incidencia Acumulada</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93012AD9-A6D4-48C4-AAAA-A2304D189270}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,6 +1288,29 @@
       <c r="A53" s="2">
         <v>44274</v>
       </c>
+      <c r="B53">
+        <v>248989</v>
+      </c>
+      <c r="C53">
+        <v>3269</v>
+      </c>
+      <c r="D53">
+        <v>205172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B54">
+        <v>251582</v>
+      </c>
+      <c r="C54">
+        <v>3302</v>
+      </c>
+      <c r="D54">
+        <v>210551</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1296,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8954D560-A495-4753-8EDD-C3E9767515C8}">
-  <dimension ref="A1:D1634"/>
+  <dimension ref="A1:D1697"/>
   <sheetViews>
-    <sheetView topLeftCell="A1608" workbookViewId="0">
-      <selection activeCell="A1634" sqref="A1634"/>
+    <sheetView tabSelected="1" topLeftCell="A1672" workbookViewId="0">
+      <selection activeCell="A1698" sqref="A1698"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24079,6 +24102,897 @@
     <row r="1634" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1634" s="2">
         <v>44274</v>
+      </c>
+      <c r="B1634" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1634">
+        <v>6846.43</v>
+      </c>
+      <c r="D1634">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1635" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1635" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1635">
+        <v>1388.94</v>
+      </c>
+      <c r="D1635">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1636" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1636" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1636">
+        <v>1346.47</v>
+      </c>
+      <c r="D1636">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1637" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1637" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1637">
+        <v>1392.35</v>
+      </c>
+      <c r="D1637">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1638" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1638" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1638">
+        <v>1570.7</v>
+      </c>
+      <c r="D1638">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1639" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1639" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1639">
+        <v>2138.75</v>
+      </c>
+      <c r="D1639">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1640" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1640" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1640">
+        <v>641.94000000000005</v>
+      </c>
+      <c r="D1640">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1641" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1641" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1641">
+        <v>940.03</v>
+      </c>
+      <c r="D1641">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1642" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1642" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1642">
+        <v>2140.5500000000002</v>
+      </c>
+      <c r="D1642">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1643" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1643" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1643">
+        <v>1665.41</v>
+      </c>
+      <c r="D1643">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1644" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1644" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1644">
+        <v>2596.73</v>
+      </c>
+      <c r="D1644">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1645" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1645" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1645">
+        <v>2777.73</v>
+      </c>
+      <c r="D1645">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1646" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1646" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1646">
+        <v>2440.13</v>
+      </c>
+      <c r="D1646">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1647" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1647" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1647">
+        <v>2177.9299999999998</v>
+      </c>
+      <c r="D1647">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1648" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1648" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1648">
+        <v>969.96</v>
+      </c>
+      <c r="D1648">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1649" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1649" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1649">
+        <v>1828.73</v>
+      </c>
+      <c r="D1649">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1650" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1650" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1650">
+        <v>1068.71</v>
+      </c>
+      <c r="D1650">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1651" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1651" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1651">
+        <v>2271.77</v>
+      </c>
+      <c r="D1651">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1652" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1652" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1652">
+        <v>2533.9699999999998</v>
+      </c>
+      <c r="D1652">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1653" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1653" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1653">
+        <v>791.73</v>
+      </c>
+      <c r="D1653">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1654" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1654" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1654">
+        <v>1165.78</v>
+      </c>
+      <c r="D1654">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1655" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1655" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1655">
+        <v>1670</v>
+      </c>
+      <c r="D1655">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1656" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1656" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1656">
+        <v>1096.52</v>
+      </c>
+      <c r="D1656">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1657" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1657" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1657">
+        <v>2061.48</v>
+      </c>
+      <c r="D1657">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1658" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1658" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1658">
+        <v>2641.39</v>
+      </c>
+      <c r="D1658">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1659" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1659" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1659">
+        <v>1980.23</v>
+      </c>
+      <c r="D1659">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1660" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1660" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1660">
+        <v>1381.85</v>
+      </c>
+      <c r="D1660">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1661" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1661" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1661">
+        <v>1977.87</v>
+      </c>
+      <c r="D1661">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1662" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1662" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1662">
+        <v>640.73</v>
+      </c>
+      <c r="D1662">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1663" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1663" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1663">
+        <v>944.47</v>
+      </c>
+      <c r="D1663">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1664" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1664">
+        <v>1485.16</v>
+      </c>
+      <c r="D1664">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1665" s="2">
+        <v>44274</v>
+      </c>
+      <c r="B1665" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1665">
+        <v>1707.6</v>
+      </c>
+      <c r="D1665">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1666" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1666" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1666">
+        <v>6937.69</v>
+      </c>
+      <c r="D1666">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1667" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1667" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1667">
+        <v>1412.79</v>
+      </c>
+      <c r="D1667">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1668" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1668" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1668">
+        <v>1351.42</v>
+      </c>
+      <c r="D1668">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1669" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1669" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1669">
+        <v>1402.39</v>
+      </c>
+      <c r="D1669">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1670" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1670" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1670">
+        <v>1579.73</v>
+      </c>
+      <c r="D1670">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1671" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1671" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1671">
+        <v>2151.8000000000002</v>
+      </c>
+      <c r="D1671">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1672" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1672" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1672">
+        <v>641.94000000000005</v>
+      </c>
+      <c r="D1672">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1673" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1673" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1673">
+        <v>943.23</v>
+      </c>
+      <c r="D1673">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1674" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1674" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1674">
+        <v>2150.9699999999998</v>
+      </c>
+      <c r="D1674">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1675" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1675" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1675">
+        <v>1675.68</v>
+      </c>
+      <c r="D1675">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1676" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1676" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1676">
+        <v>2619.08</v>
+      </c>
+      <c r="D1676">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1677" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1677" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1677">
+        <v>2810.01</v>
+      </c>
+      <c r="D1677">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1678" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1678" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1678">
+        <v>2451.31</v>
+      </c>
+      <c r="D1678">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1679" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1679" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1679">
+        <v>2186.44</v>
+      </c>
+      <c r="D1679">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1680" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1680" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1680">
+        <v>974.32</v>
+      </c>
+      <c r="D1680">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1681" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1681" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1681">
+        <v>1837.3</v>
+      </c>
+      <c r="D1681">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1682" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1682" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1682">
+        <v>1082.8900000000001</v>
+      </c>
+      <c r="D1682">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1683" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1683" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1683">
+        <v>2278.0700000000002</v>
+      </c>
+      <c r="D1683">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1684" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1684" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1684">
+        <v>2544.8200000000002</v>
+      </c>
+      <c r="D1684">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1685" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1685" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1685">
+        <v>794.4</v>
+      </c>
+      <c r="D1685">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1686" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1686" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1686">
+        <v>1177.3900000000001</v>
+      </c>
+      <c r="D1686">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1687" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1687" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1687">
+        <v>1689.85</v>
+      </c>
+      <c r="D1687">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1688" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1688" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1688">
+        <v>1114.8800000000001</v>
+      </c>
+      <c r="D1688">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1689" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1689" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1689">
+        <v>2071.35</v>
+      </c>
+      <c r="D1689">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1690" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1690">
+        <v>2658.13</v>
+      </c>
+      <c r="D1690">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1691" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1691" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1691">
+        <v>2004.68</v>
+      </c>
+      <c r="D1691">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1692" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1692" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1692">
+        <v>1394.3</v>
+      </c>
+      <c r="D1692">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1693" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1693" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1693">
+        <v>1983.61</v>
+      </c>
+      <c r="D1693">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1694" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1694" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1694">
+        <v>647.53</v>
+      </c>
+      <c r="D1694">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1695" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1695" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1695">
+        <v>957.3</v>
+      </c>
+      <c r="D1695">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1696" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1696" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1696">
+        <v>1488.83</v>
+      </c>
+      <c r="D1696">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1697" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B1697" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1697">
+        <v>1733.62</v>
+      </c>
+      <c r="D1697">
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>